<commit_message>
This commit runs and doesn't crash, but the Stop Test functionality is not working yet, due to improper use of threads.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A954DE7A-776B-44D0-B2E5-381E07A52022}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006F61B-0666-4732-926C-6BC166FCFBC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15600" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -117,9 +117,6 @@
     <t>24Vout</t>
   </si>
   <si>
-    <t>PsuaUvloRising</t>
-  </si>
-  <si>
     <t>PSUA UVLO Rising</t>
   </si>
   <si>
@@ -129,27 +126,6 @@
     <t>PSUA OVLO Rising</t>
   </si>
   <si>
-    <t>PsuaUvloFalling</t>
-  </si>
-  <si>
-    <t>PsuaOvloRising</t>
-  </si>
-  <si>
-    <t>PsuaOvloFalling</t>
-  </si>
-  <si>
-    <t>PsubUvloRising</t>
-  </si>
-  <si>
-    <t>PsubUvloFalling</t>
-  </si>
-  <si>
-    <t>PsubOvloRising</t>
-  </si>
-  <si>
-    <t>PsubOvloFalling</t>
-  </si>
-  <si>
     <t>PSUA OVLO Falling</t>
   </si>
   <si>
@@ -235,6 +211,30 @@
   </si>
   <si>
     <t>Bootstrap</t>
+  </si>
+  <si>
+    <t>Threshold1</t>
+  </si>
+  <si>
+    <t>Threshold2</t>
+  </si>
+  <si>
+    <t>Threshold3</t>
+  </si>
+  <si>
+    <t>Threshold4</t>
+  </si>
+  <si>
+    <t>Threshold5</t>
+  </si>
+  <si>
+    <t>Threshold6</t>
+  </si>
+  <si>
+    <t>Threshold7</t>
+  </si>
+  <si>
+    <t>Threshold8</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A81" sqref="A81:XFD81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,10 +649,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D2" s="2">
         <f>0.95*F2</f>
@@ -665,7 +665,9 @@
       <c r="F2" s="2">
         <v>20.18</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>-999</v>
+      </c>
       <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
@@ -676,10 +678,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D9" si="0">0.95*F3</f>
@@ -692,7 +694,9 @@
       <c r="F3" s="2">
         <v>20.18</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="3">
+        <v>-999</v>
+      </c>
       <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
@@ -703,10 +707,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -719,7 +723,9 @@
       <c r="F4" s="2">
         <v>30.2</v>
       </c>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>-999</v>
+      </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
@@ -730,10 +736,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -746,7 +752,9 @@
       <c r="F5" s="2">
         <v>30.2</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>-999</v>
+      </c>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
@@ -757,10 +765,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -773,7 +781,9 @@
       <c r="F6" s="2">
         <v>20.18</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>-999</v>
+      </c>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
@@ -784,10 +794,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -800,7 +810,9 @@
       <c r="F7" s="2">
         <v>20.18</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>-999</v>
+      </c>
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
@@ -811,10 +823,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
@@ -827,7 +839,9 @@
       <c r="F8" s="2">
         <v>30.2</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>-999</v>
+      </c>
       <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
@@ -838,10 +852,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
@@ -854,7 +868,9 @@
       <c r="F9" s="2">
         <v>30.2</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3">
+        <v>-999</v>
+      </c>
       <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
@@ -880,9 +896,11 @@
       <c r="F10" s="3">
         <v>0.05</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="3">
+        <v>-999</v>
+      </c>
       <c r="H10" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -906,9 +924,11 @@
       <c r="F11" s="3">
         <v>0.05</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="3">
+        <v>-999</v>
+      </c>
       <c r="H11" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -932,9 +952,11 @@
       <c r="F12" s="3">
         <v>0.05</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>-999</v>
+      </c>
       <c r="H12" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -958,9 +980,11 @@
       <c r="F13" s="3">
         <v>0.05</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="3">
+        <v>-999</v>
+      </c>
       <c r="H13" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -984,9 +1008,11 @@
       <c r="F14" s="3">
         <v>0.05</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="3">
+        <v>-999</v>
+      </c>
       <c r="H14" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1010,9 +1036,11 @@
       <c r="F15" s="3">
         <v>0.05</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="3">
+        <v>-999</v>
+      </c>
       <c r="H15" s="3" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1020,7 +1048,7 @@
         <v>15.01</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C16" s="3" t="str">
         <f>NoPowerState!A2</f>
@@ -1038,7 +1066,9 @@
         <f>NoPowerState!D2</f>
         <v>0</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="3">
+        <v>-999</v>
+      </c>
       <c r="H16" s="3" t="str">
         <f>NoPowerState!E2</f>
         <v>V</v>
@@ -1050,7 +1080,7 @@
         <v>15.02</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C17" s="3" t="str">
         <f>NoPowerState!A3</f>
@@ -1068,7 +1098,9 @@
         <f>NoPowerState!D3</f>
         <v>0</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="3">
+        <v>-999</v>
+      </c>
       <c r="H17" s="3" t="str">
         <f>NoPowerState!E3</f>
         <v>V</v>
@@ -1080,7 +1112,7 @@
         <v>15.03</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C18" s="3" t="str">
         <f>NoPowerState!A4</f>
@@ -1098,7 +1130,9 @@
         <f>NoPowerState!D4</f>
         <v>0</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="3">
+        <v>-999</v>
+      </c>
       <c r="H18" s="3" t="str">
         <f>NoPowerState!E4</f>
         <v>V</v>
@@ -1110,7 +1144,7 @@
         <v>15.04</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19" s="3" t="str">
         <f>NoPowerState!A5</f>
@@ -1128,7 +1162,9 @@
         <f>NoPowerState!D5</f>
         <v>0</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="3">
+        <v>-999</v>
+      </c>
       <c r="H19" s="3" t="str">
         <f>NoPowerState!E5</f>
         <v>V</v>
@@ -1140,7 +1176,7 @@
         <v>15.049999999999999</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C20" s="3" t="str">
         <f>NoPowerState!A6</f>
@@ -1158,7 +1194,9 @@
         <f>NoPowerState!D6</f>
         <v>0</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3">
+        <v>-999</v>
+      </c>
       <c r="H20" s="3" t="str">
         <f>NoPowerState!E6</f>
         <v>V</v>
@@ -1170,7 +1208,7 @@
         <v>15.059999999999999</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C21" s="3" t="str">
         <f>NoPowerState!A7</f>
@@ -1188,7 +1226,9 @@
         <f>NoPowerState!D7</f>
         <v>0</v>
       </c>
-      <c r="G21" s="3"/>
+      <c r="G21" s="3">
+        <v>-999</v>
+      </c>
       <c r="H21" s="3" t="str">
         <f>NoPowerState!E7</f>
         <v>V</v>
@@ -1200,7 +1240,7 @@
         <v>15.069999999999999</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="str">
         <f>NoPowerState!A8</f>
@@ -1218,7 +1258,9 @@
         <f>NoPowerState!D8</f>
         <v>0</v>
       </c>
-      <c r="G22" s="3"/>
+      <c r="G22" s="3">
+        <v>-999</v>
+      </c>
       <c r="H22" s="3" t="str">
         <f>NoPowerState!E8</f>
         <v>V</v>
@@ -1230,7 +1272,7 @@
         <v>15.079999999999998</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C23" s="3" t="str">
         <f>NoPowerState!A9</f>
@@ -1248,7 +1290,9 @@
         <f>NoPowerState!D9</f>
         <v>0</v>
       </c>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <v>-999</v>
+      </c>
       <c r="H23" s="3" t="str">
         <f>NoPowerState!E9</f>
         <v>V</v>
@@ -1260,7 +1304,7 @@
         <v>15.089999999999998</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="str">
         <f>NoPowerState!A10</f>
@@ -1278,7 +1322,9 @@
         <f>NoPowerState!D10</f>
         <v>0</v>
       </c>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <v>-999</v>
+      </c>
       <c r="H24" s="3" t="str">
         <f>NoPowerState!E10</f>
         <v>V</v>
@@ -1290,7 +1336,7 @@
         <v>15.099999999999998</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C25" s="3" t="str">
         <f>NoPowerState!A11</f>
@@ -1308,7 +1354,9 @@
         <f>NoPowerState!D11</f>
         <v>0</v>
       </c>
-      <c r="G25" s="3"/>
+      <c r="G25" s="3">
+        <v>-999</v>
+      </c>
       <c r="H25" s="3" t="str">
         <f>NoPowerState!E11</f>
         <v>V</v>
@@ -1320,7 +1368,7 @@
         <v>15.109999999999998</v>
       </c>
       <c r="B26" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C26" s="3" t="str">
         <f>NoPowerState!A12</f>
@@ -1338,7 +1386,9 @@
         <f>NoPowerState!D12</f>
         <v>0</v>
       </c>
-      <c r="G26" s="3"/>
+      <c r="G26" s="3">
+        <v>-999</v>
+      </c>
       <c r="H26" s="3" t="str">
         <f>NoPowerState!E12</f>
         <v>V</v>
@@ -1350,7 +1400,7 @@
         <v>15.119999999999997</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C27" s="3" t="str">
         <f>NoPowerState!A13</f>
@@ -1368,7 +1418,9 @@
         <f>NoPowerState!D13</f>
         <v>0</v>
       </c>
-      <c r="G27" s="3"/>
+      <c r="G27" s="3">
+        <v>-999</v>
+      </c>
       <c r="H27" s="3" t="str">
         <f>NoPowerState!E13</f>
         <v>V</v>
@@ -1380,7 +1432,7 @@
         <v>15.129999999999997</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C28" s="3" t="str">
         <f>NoPowerState!A14</f>
@@ -1398,7 +1450,9 @@
         <f>NoPowerState!D14</f>
         <v>0</v>
       </c>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <v>-999</v>
+      </c>
       <c r="H28" s="3" t="str">
         <f>NoPowerState!E14</f>
         <v>V</v>
@@ -1410,7 +1464,7 @@
         <v>15.139999999999997</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="str">
         <f>NoPowerState!A15</f>
@@ -1428,7 +1482,9 @@
         <f>NoPowerState!D15</f>
         <v>0</v>
       </c>
-      <c r="G29" s="3"/>
+      <c r="G29" s="3">
+        <v>-999</v>
+      </c>
       <c r="H29" s="3" t="str">
         <f>NoPowerState!E15</f>
         <v>A</v>
@@ -1439,7 +1495,7 @@
         <v>16.010000000000002</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C30" s="3" t="str">
         <f>CapsChargingState!A2</f>
@@ -1457,7 +1513,9 @@
         <f>CapsChargingState!D2</f>
         <v>24</v>
       </c>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3">
+        <v>-999</v>
+      </c>
       <c r="H30" s="3" t="str">
         <f>CapsChargingState!E2</f>
         <v>V</v>
@@ -1469,7 +1527,7 @@
         <v>16.020000000000003</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C31" s="3" t="str">
         <f>CapsChargingState!A3</f>
@@ -1487,7 +1545,9 @@
         <f>CapsChargingState!D3</f>
         <v>2.1</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3">
+        <v>-999</v>
+      </c>
       <c r="H31" s="3" t="str">
         <f>CapsChargingState!E3</f>
         <v>dv/dt</v>
@@ -1499,7 +1559,7 @@
         <v>16.030000000000005</v>
       </c>
       <c r="B32" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C32" s="3" t="str">
         <f>CapsChargingState!A4</f>
@@ -1517,7 +1577,9 @@
         <f>CapsChargingState!D4</f>
         <v>24</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <v>-999</v>
+      </c>
       <c r="H32" s="3" t="str">
         <f>CapsChargingState!E4</f>
         <v>V</v>
@@ -1528,7 +1590,7 @@
         <v>17.010000000000002</v>
       </c>
       <c r="B33" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C33" s="3" t="str">
         <f>NormalOperationState!A2</f>
@@ -1546,7 +1608,9 @@
         <f>NormalOperationState!D2</f>
         <v>24</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3">
+        <v>-999</v>
+      </c>
       <c r="H33" s="3" t="str">
         <f>NormalOperationState!E2</f>
         <v>V</v>
@@ -1558,7 +1622,7 @@
         <v>17.020000000000003</v>
       </c>
       <c r="B34" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C34" s="3" t="str">
         <f>NormalOperationState!A3</f>
@@ -1576,7 +1640,9 @@
         <f>NormalOperationState!D3</f>
         <v>24</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3">
+        <v>-999</v>
+      </c>
       <c r="H34" s="3" t="str">
         <f>NormalOperationState!E3</f>
         <v>V</v>
@@ -1588,7 +1654,7 @@
         <v>17.030000000000005</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C35" s="3" t="str">
         <f>NormalOperationState!A4</f>
@@ -1606,7 +1672,9 @@
         <f>NormalOperationState!D4</f>
         <v>0</v>
       </c>
-      <c r="G35" s="3"/>
+      <c r="G35" s="3">
+        <v>-999</v>
+      </c>
       <c r="H35" s="3" t="str">
         <f>NormalOperationState!E4</f>
         <v>V</v>
@@ -1618,7 +1686,7 @@
         <v>17.040000000000006</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C36" s="3" t="str">
         <f>NormalOperationState!A5</f>
@@ -1636,7 +1704,9 @@
         <f>NormalOperationState!D5</f>
         <v>24</v>
       </c>
-      <c r="G36" s="3"/>
+      <c r="G36" s="3">
+        <v>-999</v>
+      </c>
       <c r="H36" s="3" t="str">
         <f>NormalOperationState!E5</f>
         <v>V</v>
@@ -1648,7 +1718,7 @@
         <v>17.050000000000008</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C37" s="3" t="str">
         <f>NormalOperationState!A6</f>
@@ -1666,7 +1736,9 @@
         <f>NormalOperationState!D6</f>
         <v>0</v>
       </c>
-      <c r="G37" s="3"/>
+      <c r="G37" s="3">
+        <v>-999</v>
+      </c>
       <c r="H37" s="3" t="str">
         <f>NormalOperationState!E6</f>
         <v>V</v>
@@ -1678,7 +1750,7 @@
         <v>17.060000000000009</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3" t="str">
         <f>NormalOperationState!A7</f>
@@ -1696,7 +1768,9 @@
         <f>NormalOperationState!D7</f>
         <v>0</v>
       </c>
-      <c r="G38" s="3"/>
+      <c r="G38" s="3">
+        <v>-999</v>
+      </c>
       <c r="H38" s="3" t="str">
         <f>NormalOperationState!E7</f>
         <v>V</v>
@@ -1708,7 +1782,7 @@
         <v>17.070000000000011</v>
       </c>
       <c r="B39" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C39" s="3" t="str">
         <f>NormalOperationState!A8</f>
@@ -1726,7 +1800,9 @@
         <f>NormalOperationState!D8</f>
         <v>0</v>
       </c>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3">
+        <v>-999</v>
+      </c>
       <c r="H39" s="3" t="str">
         <f>NormalOperationState!E8</f>
         <v>V</v>
@@ -1738,7 +1814,7 @@
         <v>17.080000000000013</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C40" s="3" t="str">
         <f>NormalOperationState!A9</f>
@@ -1756,7 +1832,9 @@
         <f>NormalOperationState!D9</f>
         <v>0</v>
       </c>
-      <c r="G40" s="3"/>
+      <c r="G40" s="3">
+        <v>-999</v>
+      </c>
       <c r="H40" s="3" t="str">
         <f>NormalOperationState!E9</f>
         <v>V</v>
@@ -1768,7 +1846,7 @@
         <v>17.090000000000014</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C41" s="3" t="str">
         <f>NormalOperationState!A10</f>
@@ -1786,7 +1864,9 @@
         <f>NormalOperationState!D10</f>
         <v>315</v>
       </c>
-      <c r="G41" s="3"/>
+      <c r="G41" s="3">
+        <v>-999</v>
+      </c>
       <c r="H41" s="3" t="str">
         <f>NormalOperationState!E10</f>
         <v>V</v>
@@ -1798,7 +1878,7 @@
         <v>17.100000000000016</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C42" s="3" t="str">
         <f>NormalOperationState!A11</f>
@@ -1816,7 +1896,9 @@
         <f>NormalOperationState!D11</f>
         <v>0</v>
       </c>
-      <c r="G42" s="3"/>
+      <c r="G42" s="3">
+        <v>-999</v>
+      </c>
       <c r="H42" s="3" t="str">
         <f>NormalOperationState!E11</f>
         <v>V</v>
@@ -1828,7 +1910,7 @@
         <v>17.110000000000017</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C43" s="3" t="str">
         <f>NormalOperationState!A12</f>
@@ -1846,7 +1928,9 @@
         <f>NormalOperationState!D12</f>
         <v>800</v>
       </c>
-      <c r="G43" s="3"/>
+      <c r="G43" s="3">
+        <v>-999</v>
+      </c>
       <c r="H43" s="3" t="str">
         <f>NormalOperationState!E12</f>
         <v>V</v>
@@ -1858,7 +1942,7 @@
         <v>17.120000000000019</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C44" s="3" t="str">
         <f>NormalOperationState!A13</f>
@@ -1876,7 +1960,9 @@
         <f>NormalOperationState!D13</f>
         <v>0</v>
       </c>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3">
+        <v>-999</v>
+      </c>
       <c r="H44" s="3" t="str">
         <f>NormalOperationState!E13</f>
         <v>V</v>
@@ -1888,7 +1974,7 @@
         <v>17.13000000000002</v>
       </c>
       <c r="B45" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C45" s="3" t="str">
         <f>NormalOperationState!A14</f>
@@ -1906,7 +1992,9 @@
         <f>NormalOperationState!D14</f>
         <v>24</v>
       </c>
-      <c r="G45" s="3"/>
+      <c r="G45" s="3">
+        <v>-999</v>
+      </c>
       <c r="H45" s="3" t="str">
         <f>NormalOperationState!E14</f>
         <v>V</v>
@@ -1918,7 +2006,7 @@
         <v>17.140000000000022</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C46" s="3" t="str">
         <f>NormalOperationState!A15</f>
@@ -1936,7 +2024,9 @@
         <f>NormalOperationState!D15</f>
         <v>0</v>
       </c>
-      <c r="G46" s="3"/>
+      <c r="G46" s="3">
+        <v>-999</v>
+      </c>
       <c r="H46" s="3" t="str">
         <f>NormalOperationState!E15</f>
         <v>A</v>
@@ -1947,7 +2037,7 @@
         <v>18.010000000000002</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C47" s="3" t="str">
         <f>SPMState!A2</f>
@@ -1965,7 +2055,9 @@
         <f>SPMState!D2</f>
         <v>0</v>
       </c>
-      <c r="G47" s="3"/>
+      <c r="G47" s="3">
+        <v>-999</v>
+      </c>
       <c r="H47" s="3" t="str">
         <f>SPMState!E2</f>
         <v>V</v>
@@ -1977,7 +2069,7 @@
         <v>18.020000000000003</v>
       </c>
       <c r="B48" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C48" s="3" t="str">
         <f>SPMState!A3</f>
@@ -1994,6 +2086,9 @@
       <c r="F48" s="3">
         <f>SPMState!D3</f>
         <v>24</v>
+      </c>
+      <c r="G48" s="3">
+        <v>-999</v>
       </c>
       <c r="H48" s="3" t="str">
         <f>SPMState!E3</f>
@@ -2006,7 +2101,7 @@
         <v>18.030000000000005</v>
       </c>
       <c r="B49" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C49" s="3" t="str">
         <f>SPMState!A4</f>
@@ -2023,6 +2118,9 @@
       <c r="F49" s="3">
         <f>SPMState!D4</f>
         <v>0</v>
+      </c>
+      <c r="G49" s="3">
+        <v>-999</v>
       </c>
       <c r="H49" s="3" t="str">
         <f>SPMState!E4</f>
@@ -2035,7 +2133,7 @@
         <v>18.040000000000006</v>
       </c>
       <c r="B50" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C50" s="3" t="str">
         <f>SPMState!A5</f>
@@ -2052,6 +2150,9 @@
       <c r="F50" s="3">
         <f>SPMState!D5</f>
         <v>24</v>
+      </c>
+      <c r="G50" s="3">
+        <v>-999</v>
       </c>
       <c r="H50" s="3" t="str">
         <f>SPMState!E5</f>
@@ -2064,7 +2165,7 @@
         <v>18.050000000000008</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3" t="str">
         <f>SPMState!A6</f>
@@ -2081,6 +2182,9 @@
       <c r="F51" s="3">
         <f>SPMState!D6</f>
         <v>5</v>
+      </c>
+      <c r="G51" s="3">
+        <v>-999</v>
       </c>
       <c r="H51" s="3" t="str">
         <f>SPMState!E6</f>
@@ -2093,7 +2197,7 @@
         <v>18.060000000000009</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C52" s="3" t="str">
         <f>SPMState!A7</f>
@@ -2110,6 +2214,9 @@
       <c r="F52" s="3">
         <f>SPMState!D7</f>
         <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>-999</v>
       </c>
       <c r="H52" s="3" t="str">
         <f>SPMState!E7</f>
@@ -2122,7 +2229,7 @@
         <v>18.070000000000011</v>
       </c>
       <c r="B53" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C53" s="3" t="str">
         <f>SPMState!A8</f>
@@ -2139,6 +2246,9 @@
       <c r="F53" s="3">
         <f>SPMState!D8</f>
         <v>5</v>
+      </c>
+      <c r="G53" s="3">
+        <v>-999</v>
       </c>
       <c r="H53" s="3" t="str">
         <f>SPMState!E8</f>
@@ -2151,7 +2261,7 @@
         <v>18.080000000000013</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C54" s="3" t="str">
         <f>SPMState!A9</f>
@@ -2168,6 +2278,9 @@
       <c r="F54" s="3">
         <f>SPMState!D9</f>
         <v>0</v>
+      </c>
+      <c r="G54" s="3">
+        <v>-999</v>
       </c>
       <c r="H54" s="3" t="str">
         <f>SPMState!E9</f>
@@ -2180,7 +2293,7 @@
         <v>18.090000000000014</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C55" s="3" t="str">
         <f>SPMState!A10</f>
@@ -2197,6 +2310,9 @@
       <c r="F55" s="3">
         <f>SPMState!D10</f>
         <v>240</v>
+      </c>
+      <c r="G55" s="3">
+        <v>-999</v>
       </c>
       <c r="H55" s="3" t="str">
         <f>SPMState!E10</f>
@@ -2209,7 +2325,7 @@
         <v>18.100000000000016</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C56" s="3" t="str">
         <f>SPMState!A11</f>
@@ -2226,6 +2342,9 @@
       <c r="F56" s="3">
         <f>SPMState!D11</f>
         <v>240</v>
+      </c>
+      <c r="G56" s="3">
+        <v>-999</v>
       </c>
       <c r="H56" s="3" t="str">
         <f>SPMState!E11</f>
@@ -2238,7 +2357,7 @@
         <v>18.110000000000017</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C57" s="3" t="str">
         <f>SPMState!A12</f>
@@ -2255,6 +2374,9 @@
       <c r="F57" s="3">
         <f>SPMState!D12</f>
         <v>800</v>
+      </c>
+      <c r="G57" s="3">
+        <v>-999</v>
       </c>
       <c r="H57" s="3" t="str">
         <f>SPMState!E12</f>
@@ -2267,7 +2389,7 @@
         <v>18.120000000000019</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C58" s="3" t="str">
         <f>SPMState!A13</f>
@@ -2284,6 +2406,9 @@
       <c r="F58" s="3">
         <f>SPMState!D13</f>
         <v>16</v>
+      </c>
+      <c r="G58" s="3">
+        <v>-999</v>
       </c>
       <c r="H58" s="3" t="str">
         <f>SPMState!E13</f>
@@ -2296,7 +2421,7 @@
         <v>18.13000000000002</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C59" s="3" t="str">
         <f>SPMState!A14</f>
@@ -2313,6 +2438,9 @@
       <c r="F59" s="3">
         <f>SPMState!D14</f>
         <v>24</v>
+      </c>
+      <c r="G59" s="3">
+        <v>-999</v>
       </c>
       <c r="H59" s="3" t="str">
         <f>SPMState!E14</f>
@@ -2325,7 +2453,7 @@
         <v>18.140000000000022</v>
       </c>
       <c r="B60" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C60" s="3" t="str">
         <f>SPMState!A15</f>
@@ -2342,6 +2470,9 @@
       <c r="F60" s="3">
         <f>SPMState!D15</f>
         <v>0</v>
+      </c>
+      <c r="G60" s="3">
+        <v>-999</v>
       </c>
       <c r="H60" s="3" t="str">
         <f>SPMState!E15</f>
@@ -2354,7 +2485,7 @@
         <v>18.150000000000023</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C61" s="3" t="str">
         <f>SPMState!A16</f>
@@ -2372,6 +2503,9 @@
         <f>SPMState!D16</f>
         <v>95</v>
       </c>
+      <c r="G61" s="3">
+        <v>-999</v>
+      </c>
       <c r="H61" s="3" t="str">
         <f>SPMState!E16</f>
         <v>%</v>
@@ -2382,7 +2516,7 @@
         <v>19.010000000000002</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C62" s="3" t="str">
         <f>NoPowerState!A2</f>
@@ -2399,6 +2533,9 @@
       <c r="F62" s="3">
         <f>NoPowerState!D2</f>
         <v>0</v>
+      </c>
+      <c r="G62" s="3">
+        <v>-999</v>
       </c>
       <c r="H62" s="3" t="str">
         <f>NoPowerState!E2</f>
@@ -2411,7 +2548,7 @@
         <v>19.020000000000003</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C63" s="3" t="str">
         <f>NoPowerState!A3</f>
@@ -2428,6 +2565,9 @@
       <c r="F63" s="3">
         <f>NoPowerState!D3</f>
         <v>0</v>
+      </c>
+      <c r="G63" s="3">
+        <v>-999</v>
       </c>
       <c r="H63" s="3" t="str">
         <f>NoPowerState!E3</f>
@@ -2440,7 +2580,7 @@
         <v>19.030000000000005</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C64" s="3" t="str">
         <f>NoPowerState!A4</f>
@@ -2457,6 +2597,9 @@
       <c r="F64" s="3">
         <f>NoPowerState!D4</f>
         <v>0</v>
+      </c>
+      <c r="G64" s="3">
+        <v>-999</v>
       </c>
       <c r="H64" s="3" t="str">
         <f>NoPowerState!E4</f>
@@ -2469,7 +2612,7 @@
         <v>19.040000000000006</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C65" s="3" t="str">
         <f>NoPowerState!A5</f>
@@ -2486,6 +2629,9 @@
       <c r="F65" s="3">
         <f>NoPowerState!D5</f>
         <v>0</v>
+      </c>
+      <c r="G65" s="3">
+        <v>-999</v>
       </c>
       <c r="H65" s="3" t="str">
         <f>NoPowerState!E5</f>
@@ -2498,7 +2644,7 @@
         <v>19.050000000000008</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C66" s="3" t="str">
         <f>NoPowerState!A6</f>
@@ -2515,6 +2661,9 @@
       <c r="F66" s="3">
         <f>NoPowerState!D6</f>
         <v>0</v>
+      </c>
+      <c r="G66" s="3">
+        <v>-999</v>
       </c>
       <c r="H66" s="3" t="str">
         <f>NoPowerState!E6</f>
@@ -2527,7 +2676,7 @@
         <v>19.060000000000009</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C67" s="3" t="str">
         <f>NoPowerState!A7</f>
@@ -2544,6 +2693,9 @@
       <c r="F67" s="3">
         <f>NoPowerState!D7</f>
         <v>0</v>
+      </c>
+      <c r="G67" s="3">
+        <v>-999</v>
       </c>
       <c r="H67" s="3" t="str">
         <f>NoPowerState!E7</f>
@@ -2556,7 +2708,7 @@
         <v>19.070000000000011</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C68" s="3" t="str">
         <f>NoPowerState!A8</f>
@@ -2573,6 +2725,9 @@
       <c r="F68" s="3">
         <f>NoPowerState!D8</f>
         <v>0</v>
+      </c>
+      <c r="G68" s="3">
+        <v>-999</v>
       </c>
       <c r="H68" s="3" t="str">
         <f>NoPowerState!E8</f>
@@ -2585,7 +2740,7 @@
         <v>19.080000000000013</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C69" s="3" t="str">
         <f>NoPowerState!A9</f>
@@ -2602,6 +2757,9 @@
       <c r="F69" s="3">
         <f>NoPowerState!D9</f>
         <v>0</v>
+      </c>
+      <c r="G69" s="3">
+        <v>-999</v>
       </c>
       <c r="H69" s="3" t="str">
         <f>NoPowerState!E9</f>
@@ -2614,7 +2772,7 @@
         <v>19.090000000000014</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C70" s="3" t="str">
         <f>NoPowerState!A10</f>
@@ -2631,6 +2789,9 @@
       <c r="F70" s="3">
         <f>NoPowerState!D10</f>
         <v>0</v>
+      </c>
+      <c r="G70" s="3">
+        <v>-999</v>
       </c>
       <c r="H70" s="3" t="str">
         <f>NoPowerState!E10</f>
@@ -2643,7 +2804,7 @@
         <v>19.100000000000016</v>
       </c>
       <c r="B71" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C71" s="3" t="str">
         <f>NoPowerState!A11</f>
@@ -2660,6 +2821,9 @@
       <c r="F71" s="3">
         <f>NoPowerState!D11</f>
         <v>0</v>
+      </c>
+      <c r="G71" s="3">
+        <v>-999</v>
       </c>
       <c r="H71" s="3" t="str">
         <f>NoPowerState!E11</f>
@@ -2672,7 +2836,7 @@
         <v>19.110000000000017</v>
       </c>
       <c r="B72" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C72" s="3" t="str">
         <f>NoPowerState!A12</f>
@@ -2689,6 +2853,9 @@
       <c r="F72" s="3">
         <f>NoPowerState!D12</f>
         <v>0</v>
+      </c>
+      <c r="G72" s="3">
+        <v>-999</v>
       </c>
       <c r="H72" s="3" t="str">
         <f>NoPowerState!E12</f>
@@ -2701,7 +2868,7 @@
         <v>19.120000000000019</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C73" s="3" t="str">
         <f>NoPowerState!A13</f>
@@ -2718,6 +2885,9 @@
       <c r="F73" s="3">
         <f>NoPowerState!D13</f>
         <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>-999</v>
       </c>
       <c r="H73" s="3" t="str">
         <f>NoPowerState!E13</f>
@@ -2730,7 +2900,7 @@
         <v>19.13000000000002</v>
       </c>
       <c r="B74" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C74" s="3" t="str">
         <f>NoPowerState!A14</f>
@@ -2747,6 +2917,9 @@
       <c r="F74" s="3">
         <f>NoPowerState!D14</f>
         <v>0</v>
+      </c>
+      <c r="G74" s="3">
+        <v>-999</v>
       </c>
       <c r="H74" s="3" t="str">
         <f>NoPowerState!E14</f>
@@ -2759,7 +2932,7 @@
         <v>19.140000000000022</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C75" s="3" t="str">
         <f>NoPowerState!A15</f>
@@ -2777,6 +2950,9 @@
         <f>NoPowerState!D15</f>
         <v>0</v>
       </c>
+      <c r="G75" s="3">
+        <v>-999</v>
+      </c>
       <c r="H75" s="3" t="str">
         <f>NoPowerState!E15</f>
         <v>A</v>
@@ -2787,7 +2963,7 @@
         <v>20.010000000000002</v>
       </c>
       <c r="B76" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C76" s="3" t="str">
         <f>BootstrapState!A2</f>
@@ -2804,6 +2980,9 @@
       <c r="F76" s="3">
         <f>BootstrapState!D2</f>
         <v>20</v>
+      </c>
+      <c r="G76" s="3">
+        <v>-999</v>
       </c>
       <c r="H76" s="3" t="str">
         <f>BootstrapState!E2</f>
@@ -2816,7 +2995,7 @@
         <v>20.020000000000003</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C77" s="3" t="str">
         <f>BootstrapState!A3</f>
@@ -2833,6 +3012,9 @@
       <c r="F77" s="3">
         <f>BootstrapState!D3</f>
         <v>20</v>
+      </c>
+      <c r="G77" s="3">
+        <v>-999</v>
       </c>
       <c r="H77" s="3" t="str">
         <f>BootstrapState!E3</f>
@@ -2845,7 +3027,7 @@
         <v>20.030000000000005</v>
       </c>
       <c r="B78" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C78" s="3" t="str">
         <f>BootstrapState!A4</f>
@@ -2862,6 +3044,9 @@
       <c r="F78" s="3">
         <f>BootstrapState!D4</f>
         <v>290</v>
+      </c>
+      <c r="G78" s="3">
+        <v>-999</v>
       </c>
       <c r="H78" s="3" t="str">
         <f>BootstrapState!E4</f>
@@ -2874,7 +3059,7 @@
         <v>20.040000000000006</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C79" s="3" t="str">
         <f>BootstrapState!A5</f>
@@ -2891,6 +3076,9 @@
       <c r="F79" s="3">
         <f>BootstrapState!D5</f>
         <v>16</v>
+      </c>
+      <c r="G79" s="3">
+        <v>-999</v>
       </c>
       <c r="H79" s="3" t="str">
         <f>BootstrapState!E5</f>
@@ -2903,7 +3091,7 @@
         <v>20.050000000000008</v>
       </c>
       <c r="B80" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C80" s="3" t="str">
         <f>BootstrapState!A6</f>
@@ -2921,6 +3109,9 @@
         <f>BootstrapState!D6</f>
         <v>24</v>
       </c>
+      <c r="G80" s="3">
+        <v>-999</v>
+      </c>
       <c r="H80" s="3" t="str">
         <f>BootstrapState!E6</f>
         <v>V</v>
@@ -2931,7 +3122,7 @@
         <v>21.01</v>
       </c>
       <c r="B81" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C81" s="3" t="str">
         <f>SPMState!A2</f>
@@ -2948,6 +3139,9 @@
       <c r="F81" s="3">
         <f>SPMState!D2</f>
         <v>0</v>
+      </c>
+      <c r="G81" s="3">
+        <v>-999</v>
       </c>
       <c r="H81" s="3" t="str">
         <f>SPMState!E2</f>
@@ -2960,7 +3154,7 @@
         <v>21.020000000000003</v>
       </c>
       <c r="B82" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C82" s="3" t="str">
         <f>SPMState!A3</f>
@@ -2977,6 +3171,9 @@
       <c r="F82" s="3">
         <f>SPMState!D3</f>
         <v>24</v>
+      </c>
+      <c r="G82" s="3">
+        <v>-999</v>
       </c>
       <c r="H82" s="3" t="str">
         <f>SPMState!E3</f>
@@ -2989,7 +3186,7 @@
         <v>21.030000000000005</v>
       </c>
       <c r="B83" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C83" s="3" t="str">
         <f>SPMState!A4</f>
@@ -3006,6 +3203,9 @@
       <c r="F83" s="3">
         <f>SPMState!D4</f>
         <v>0</v>
+      </c>
+      <c r="G83" s="3">
+        <v>-999</v>
       </c>
       <c r="H83" s="3" t="str">
         <f>SPMState!E4</f>
@@ -3018,7 +3218,7 @@
         <v>21.040000000000006</v>
       </c>
       <c r="B84" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C84" s="3" t="str">
         <f>SPMState!A5</f>
@@ -3035,6 +3235,9 @@
       <c r="F84" s="3">
         <f>SPMState!D5</f>
         <v>24</v>
+      </c>
+      <c r="G84" s="3">
+        <v>-999</v>
       </c>
       <c r="H84" s="3" t="str">
         <f>SPMState!E5</f>
@@ -3047,7 +3250,7 @@
         <v>21.050000000000008</v>
       </c>
       <c r="B85" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C85" s="3" t="str">
         <f>SPMState!A6</f>
@@ -3064,6 +3267,9 @@
       <c r="F85" s="3">
         <f>SPMState!D6</f>
         <v>5</v>
+      </c>
+      <c r="G85" s="3">
+        <v>-999</v>
       </c>
       <c r="H85" s="3" t="str">
         <f>SPMState!E6</f>
@@ -3076,7 +3282,7 @@
         <v>21.060000000000009</v>
       </c>
       <c r="B86" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C86" s="3" t="str">
         <f>SPMState!A7</f>
@@ -3093,6 +3299,9 @@
       <c r="F86" s="3">
         <f>SPMState!D7</f>
         <v>0</v>
+      </c>
+      <c r="G86" s="3">
+        <v>-999</v>
       </c>
       <c r="H86" s="3" t="str">
         <f>SPMState!E7</f>
@@ -3105,7 +3314,7 @@
         <v>21.070000000000011</v>
       </c>
       <c r="B87" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C87" s="3" t="str">
         <f>SPMState!A8</f>
@@ -3122,6 +3331,9 @@
       <c r="F87" s="3">
         <f>SPMState!D8</f>
         <v>5</v>
+      </c>
+      <c r="G87" s="3">
+        <v>-999</v>
       </c>
       <c r="H87" s="3" t="str">
         <f>SPMState!E8</f>
@@ -3134,7 +3346,7 @@
         <v>21.080000000000013</v>
       </c>
       <c r="B88" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C88" s="3" t="str">
         <f>SPMState!A9</f>
@@ -3151,6 +3363,9 @@
       <c r="F88" s="3">
         <f>SPMState!D9</f>
         <v>0</v>
+      </c>
+      <c r="G88" s="3">
+        <v>-999</v>
       </c>
       <c r="H88" s="3" t="str">
         <f>SPMState!E9</f>
@@ -3163,7 +3378,7 @@
         <v>21.090000000000014</v>
       </c>
       <c r="B89" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C89" s="3" t="str">
         <f>SPMState!A10</f>
@@ -3180,6 +3395,9 @@
       <c r="F89" s="3">
         <f>SPMState!D10</f>
         <v>240</v>
+      </c>
+      <c r="G89" s="3">
+        <v>-999</v>
       </c>
       <c r="H89" s="3" t="str">
         <f>SPMState!E10</f>
@@ -3192,7 +3410,7 @@
         <v>21.100000000000016</v>
       </c>
       <c r="B90" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C90" s="3" t="str">
         <f>SPMState!A11</f>
@@ -3209,6 +3427,9 @@
       <c r="F90" s="3">
         <f>SPMState!D11</f>
         <v>240</v>
+      </c>
+      <c r="G90" s="3">
+        <v>-999</v>
       </c>
       <c r="H90" s="3" t="str">
         <f>SPMState!E11</f>
@@ -3221,7 +3442,7 @@
         <v>21.110000000000017</v>
       </c>
       <c r="B91" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C91" s="3" t="str">
         <f>SPMState!A12</f>
@@ -3238,6 +3459,9 @@
       <c r="F91" s="3">
         <f>SPMState!D12</f>
         <v>800</v>
+      </c>
+      <c r="G91" s="3">
+        <v>-999</v>
       </c>
       <c r="H91" s="3" t="str">
         <f>SPMState!E12</f>
@@ -3250,7 +3474,7 @@
         <v>21.120000000000019</v>
       </c>
       <c r="B92" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C92" s="3" t="str">
         <f>SPMState!A13</f>
@@ -3267,6 +3491,9 @@
       <c r="F92" s="3">
         <f>SPMState!D13</f>
         <v>16</v>
+      </c>
+      <c r="G92" s="3">
+        <v>-999</v>
       </c>
       <c r="H92" s="3" t="str">
         <f>SPMState!E13</f>
@@ -3279,7 +3506,7 @@
         <v>21.13000000000002</v>
       </c>
       <c r="B93" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C93" s="3" t="str">
         <f>SPMState!A14</f>
@@ -3296,6 +3523,9 @@
       <c r="F93" s="3">
         <f>SPMState!D14</f>
         <v>24</v>
+      </c>
+      <c r="G93" s="3">
+        <v>-999</v>
       </c>
       <c r="H93" s="3" t="str">
         <f>SPMState!E14</f>
@@ -3308,7 +3538,7 @@
         <v>21.140000000000022</v>
       </c>
       <c r="B94" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C94" s="3" t="str">
         <f>SPMState!A15</f>
@@ -3325,6 +3555,9 @@
       <c r="F94" s="3">
         <f>SPMState!D15</f>
         <v>0</v>
+      </c>
+      <c r="G94" s="3">
+        <v>-999</v>
       </c>
       <c r="H94" s="3" t="str">
         <f>SPMState!E15</f>
@@ -3337,7 +3570,7 @@
         <v>21.150000000000023</v>
       </c>
       <c r="B95" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C95" s="3" t="str">
         <f>SPMState!A16</f>
@@ -3354,6 +3587,9 @@
       <c r="F95" s="3">
         <f>SPMState!D16</f>
         <v>95</v>
+      </c>
+      <c r="G95" s="3">
+        <v>-999</v>
       </c>
       <c r="H95" s="3" t="str">
         <f>SPMState!E16</f>
@@ -3398,7 +3634,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3">
         <v>-0.5</v>
@@ -3415,7 +3651,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3">
         <v>-0.5</v>
@@ -3432,7 +3668,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3">
         <v>-0.5</v>
@@ -3466,7 +3702,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3">
         <v>-0.5</v>
@@ -3483,7 +3719,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3">
         <v>-0.5</v>
@@ -3500,7 +3736,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>-0.5</v>
@@ -3517,7 +3753,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3">
         <v>-0.5</v>
@@ -3534,7 +3770,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>-0.5</v>
@@ -3551,7 +3787,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>-0.5</v>
@@ -3568,7 +3804,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3">
         <v>-0.5</v>
@@ -3585,7 +3821,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3">
         <v>-0.5</v>
@@ -3602,7 +3838,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>-0.5</v>
@@ -3619,7 +3855,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3">
         <v>-0.1</v>
@@ -3631,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3671,7 +3907,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3">
         <v>23</v>
@@ -3688,7 +3924,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -3705,7 +3941,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -3739,7 +3975,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3">
         <v>-0.5</v>
@@ -3756,7 +3992,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3">
         <v>-0.5</v>
@@ -3773,7 +4009,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>-0.5</v>
@@ -3790,7 +4026,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3">
         <v>-0.5</v>
@@ -3807,7 +4043,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>310</v>
@@ -3824,7 +4060,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>-0.5</v>
@@ -3841,7 +4077,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3">
         <v>750</v>
@@ -3858,7 +4094,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3">
         <v>-0.5</v>
@@ -3875,7 +4111,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>23</v>
@@ -3892,7 +4128,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3">
         <v>-0.1</v>
@@ -3904,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -3958,7 +4194,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -3970,12 +4206,12 @@
         <v>2.1</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B4" s="3">
         <v>23</v>
@@ -4029,7 +4265,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3">
         <v>0</v>
@@ -4046,7 +4282,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -4063,7 +4299,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -4097,7 +4333,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3">
         <v>4.9000000000000004</v>
@@ -4114,7 +4350,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -4131,7 +4367,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8" s="3">
         <v>4.9000000000000004</v>
@@ -4148,7 +4384,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -4165,7 +4401,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>235</v>
@@ -4182,7 +4418,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3">
         <v>235</v>
@@ -4199,7 +4435,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12" s="3">
         <v>799</v>
@@ -4216,7 +4452,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13" s="3">
         <v>15.5</v>
@@ -4233,7 +4469,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3">
         <v>23</v>
@@ -4250,7 +4486,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -4262,12 +4498,12 @@
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B16" s="3">
         <v>85</v>
@@ -4319,7 +4555,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -4331,12 +4567,12 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B3" s="3">
         <v>15</v>
@@ -4348,12 +4584,12 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B4" s="3">
         <v>285</v>
@@ -4370,7 +4606,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B5" s="3">
         <v>15.5</v>
@@ -4387,7 +4623,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3">
         <v>23</v>
@@ -4432,21 +4668,21 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <v>201</v>
@@ -4460,7 +4696,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>202</v>
@@ -4474,7 +4710,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>203</v>
@@ -4502,7 +4738,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>205</v>
@@ -4516,7 +4752,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B7">
         <v>206</v>
@@ -4530,7 +4766,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>207</v>
@@ -4544,7 +4780,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>208</v>
@@ -4558,7 +4794,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B10">
         <v>210</v>
@@ -4572,7 +4808,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B11">
         <v>211</v>
@@ -4586,7 +4822,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B12">
         <v>212</v>
@@ -4600,7 +4836,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="B13">
         <v>213</v>
@@ -4614,7 +4850,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="B14">
         <v>214</v>
@@ -4628,7 +4864,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="B15">
         <v>215</v>

</xml_diff>

<commit_message>
Ivan and I reimplemented get_current_protection_state to detect current control mode. I fixed the HV diode tests and those all run well. Working on threshold checks.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7006F61B-0666-4732-926C-6BC166FCFBC2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DCA6A9-A019-4DB4-8400-0AB496F84914}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="1455" yWindow="1455" windowWidth="21600" windowHeight="11850" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,9 +665,7 @@
       <c r="F2" s="2">
         <v>20.18</v>
       </c>
-      <c r="G2" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
@@ -694,9 +692,7 @@
       <c r="F3" s="2">
         <v>20.18</v>
       </c>
-      <c r="G3" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
@@ -723,9 +719,7 @@
       <c r="F4" s="2">
         <v>30.2</v>
       </c>
-      <c r="G4" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
@@ -752,9 +746,7 @@
       <c r="F5" s="2">
         <v>30.2</v>
       </c>
-      <c r="G5" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
@@ -781,9 +773,7 @@
       <c r="F6" s="2">
         <v>20.18</v>
       </c>
-      <c r="G6" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
         <v>9</v>
       </c>
@@ -810,9 +800,7 @@
       <c r="F7" s="2">
         <v>20.18</v>
       </c>
-      <c r="G7" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
         <v>9</v>
       </c>
@@ -839,9 +827,7 @@
       <c r="F8" s="2">
         <v>30.2</v>
       </c>
-      <c r="G8" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
         <v>9</v>
       </c>
@@ -868,9 +854,7 @@
       <c r="F9" s="2">
         <v>30.2</v>
       </c>
-      <c r="G9" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
         <v>9</v>
       </c>
@@ -890,15 +874,12 @@
         <v>0</v>
       </c>
       <c r="E10" s="3">
-        <f t="shared" ref="E10:E15" si="3">1.1*F10</f>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F10" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G10" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
         <v>35</v>
       </c>
@@ -918,15 +899,12 @@
         <v>0</v>
       </c>
       <c r="E11" s="3">
-        <f t="shared" si="3"/>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F11" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G11" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
@@ -946,15 +924,12 @@
         <v>0</v>
       </c>
       <c r="E12" s="3">
-        <f t="shared" si="3"/>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F12" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G12" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
         <v>35</v>
       </c>
@@ -974,15 +949,12 @@
         <v>0</v>
       </c>
       <c r="E13" s="3">
-        <f t="shared" si="3"/>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F13" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G13" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
         <v>35</v>
       </c>
@@ -1002,15 +974,12 @@
         <v>0</v>
       </c>
       <c r="E14" s="3">
-        <f t="shared" si="3"/>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F14" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G14" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
         <v>35</v>
       </c>
@@ -1030,15 +999,12 @@
         <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>5.5000000000000007E-2</v>
+        <v>1E-3</v>
       </c>
       <c r="F15" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="G15" s="3">
-        <v>-999</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1066,9 +1032,7 @@
         <f>NoPowerState!D2</f>
         <v>0</v>
       </c>
-      <c r="G16" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3" t="str">
         <f>NoPowerState!E2</f>
         <v>V</v>
@@ -1098,9 +1062,7 @@
         <f>NoPowerState!D3</f>
         <v>0</v>
       </c>
-      <c r="G17" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="3" t="str">
         <f>NoPowerState!E3</f>
         <v>V</v>
@@ -1108,7 +1070,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" ref="A18:A29" si="4">A17+0.01</f>
+        <f t="shared" ref="A18:A29" si="3">A17+0.01</f>
         <v>15.03</v>
       </c>
       <c r="B18" t="s">
@@ -1130,9 +1092,7 @@
         <f>NoPowerState!D4</f>
         <v>0</v>
       </c>
-      <c r="G18" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3" t="str">
         <f>NoPowerState!E4</f>
         <v>V</v>
@@ -1140,7 +1100,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.04</v>
       </c>
       <c r="B19" t="s">
@@ -1162,9 +1122,7 @@
         <f>NoPowerState!D5</f>
         <v>0</v>
       </c>
-      <c r="G19" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G19" s="3"/>
       <c r="H19" s="3" t="str">
         <f>NoPowerState!E5</f>
         <v>V</v>
@@ -1172,7 +1130,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.049999999999999</v>
       </c>
       <c r="B20" t="s">
@@ -1194,9 +1152,7 @@
         <f>NoPowerState!D6</f>
         <v>0</v>
       </c>
-      <c r="G20" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G20" s="3"/>
       <c r="H20" s="3" t="str">
         <f>NoPowerState!E6</f>
         <v>V</v>
@@ -1204,7 +1160,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.059999999999999</v>
       </c>
       <c r="B21" t="s">
@@ -1226,9 +1182,7 @@
         <f>NoPowerState!D7</f>
         <v>0</v>
       </c>
-      <c r="G21" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="3" t="str">
         <f>NoPowerState!E7</f>
         <v>V</v>
@@ -1236,7 +1190,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.069999999999999</v>
       </c>
       <c r="B22" t="s">
@@ -1258,9 +1212,7 @@
         <f>NoPowerState!D8</f>
         <v>0</v>
       </c>
-      <c r="G22" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3" t="str">
         <f>NoPowerState!E8</f>
         <v>V</v>
@@ -1268,7 +1220,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.079999999999998</v>
       </c>
       <c r="B23" t="s">
@@ -1290,9 +1242,7 @@
         <f>NoPowerState!D9</f>
         <v>0</v>
       </c>
-      <c r="G23" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="3" t="str">
         <f>NoPowerState!E9</f>
         <v>V</v>
@@ -1300,7 +1250,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.089999999999998</v>
       </c>
       <c r="B24" t="s">
@@ -1322,9 +1272,7 @@
         <f>NoPowerState!D10</f>
         <v>0</v>
       </c>
-      <c r="G24" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G24" s="3"/>
       <c r="H24" s="3" t="str">
         <f>NoPowerState!E10</f>
         <v>V</v>
@@ -1332,7 +1280,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.099999999999998</v>
       </c>
       <c r="B25" t="s">
@@ -1354,9 +1302,7 @@
         <f>NoPowerState!D11</f>
         <v>0</v>
       </c>
-      <c r="G25" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G25" s="3"/>
       <c r="H25" s="3" t="str">
         <f>NoPowerState!E11</f>
         <v>V</v>
@@ -1364,7 +1310,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.109999999999998</v>
       </c>
       <c r="B26" t="s">
@@ -1386,9 +1332,7 @@
         <f>NoPowerState!D12</f>
         <v>0</v>
       </c>
-      <c r="G26" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G26" s="3"/>
       <c r="H26" s="3" t="str">
         <f>NoPowerState!E12</f>
         <v>V</v>
@@ -1418,9 +1362,7 @@
         <f>NoPowerState!D13</f>
         <v>0</v>
       </c>
-      <c r="G27" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G27" s="3"/>
       <c r="H27" s="3" t="str">
         <f>NoPowerState!E13</f>
         <v>V</v>
@@ -1428,7 +1370,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.129999999999997</v>
       </c>
       <c r="B28" t="s">
@@ -1450,9 +1392,7 @@
         <f>NoPowerState!D14</f>
         <v>0</v>
       </c>
-      <c r="G28" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G28" s="3"/>
       <c r="H28" s="3" t="str">
         <f>NoPowerState!E14</f>
         <v>V</v>
@@ -1460,7 +1400,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15.139999999999997</v>
       </c>
       <c r="B29" t="s">
@@ -1482,9 +1422,7 @@
         <f>NoPowerState!D15</f>
         <v>0</v>
       </c>
-      <c r="G29" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G29" s="3"/>
       <c r="H29" s="3" t="str">
         <f>NoPowerState!E15</f>
         <v>A</v>
@@ -1513,9 +1451,7 @@
         <f>CapsChargingState!D2</f>
         <v>24</v>
       </c>
-      <c r="G30" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G30" s="3"/>
       <c r="H30" s="3" t="str">
         <f>CapsChargingState!E2</f>
         <v>V</v>
@@ -1545,9 +1481,7 @@
         <f>CapsChargingState!D3</f>
         <v>2.1</v>
       </c>
-      <c r="G31" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G31" s="3"/>
       <c r="H31" s="3" t="str">
         <f>CapsChargingState!E3</f>
         <v>dv/dt</v>
@@ -1577,9 +1511,7 @@
         <f>CapsChargingState!D4</f>
         <v>24</v>
       </c>
-      <c r="G32" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G32" s="3"/>
       <c r="H32" s="3" t="str">
         <f>CapsChargingState!E4</f>
         <v>V</v>
@@ -1608,9 +1540,7 @@
         <f>NormalOperationState!D2</f>
         <v>24</v>
       </c>
-      <c r="G33" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G33" s="3"/>
       <c r="H33" s="3" t="str">
         <f>NormalOperationState!E2</f>
         <v>V</v>
@@ -1640,9 +1570,7 @@
         <f>NormalOperationState!D3</f>
         <v>24</v>
       </c>
-      <c r="G34" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G34" s="3"/>
       <c r="H34" s="3" t="str">
         <f>NormalOperationState!E3</f>
         <v>V</v>
@@ -1650,7 +1578,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <f t="shared" ref="A35:A46" si="5">A34+0.01</f>
+        <f t="shared" ref="A35:A46" si="4">A34+0.01</f>
         <v>17.030000000000005</v>
       </c>
       <c r="B35" t="s">
@@ -1672,9 +1600,7 @@
         <f>NormalOperationState!D4</f>
         <v>0</v>
       </c>
-      <c r="G35" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G35" s="3"/>
       <c r="H35" s="3" t="str">
         <f>NormalOperationState!E4</f>
         <v>V</v>
@@ -1682,7 +1608,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.040000000000006</v>
       </c>
       <c r="B36" t="s">
@@ -1704,9 +1630,7 @@
         <f>NormalOperationState!D5</f>
         <v>24</v>
       </c>
-      <c r="G36" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G36" s="3"/>
       <c r="H36" s="3" t="str">
         <f>NormalOperationState!E5</f>
         <v>V</v>
@@ -1714,7 +1638,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.050000000000008</v>
       </c>
       <c r="B37" t="s">
@@ -1736,9 +1660,7 @@
         <f>NormalOperationState!D6</f>
         <v>0</v>
       </c>
-      <c r="G37" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G37" s="3"/>
       <c r="H37" s="3" t="str">
         <f>NormalOperationState!E6</f>
         <v>V</v>
@@ -1746,7 +1668,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.060000000000009</v>
       </c>
       <c r="B38" t="s">
@@ -1768,9 +1690,7 @@
         <f>NormalOperationState!D7</f>
         <v>0</v>
       </c>
-      <c r="G38" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="3" t="str">
         <f>NormalOperationState!E7</f>
         <v>V</v>
@@ -1778,7 +1698,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.070000000000011</v>
       </c>
       <c r="B39" t="s">
@@ -1800,9 +1720,7 @@
         <f>NormalOperationState!D8</f>
         <v>0</v>
       </c>
-      <c r="G39" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G39" s="3"/>
       <c r="H39" s="3" t="str">
         <f>NormalOperationState!E8</f>
         <v>V</v>
@@ -1810,7 +1728,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.080000000000013</v>
       </c>
       <c r="B40" t="s">
@@ -1832,9 +1750,7 @@
         <f>NormalOperationState!D9</f>
         <v>0</v>
       </c>
-      <c r="G40" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G40" s="3"/>
       <c r="H40" s="3" t="str">
         <f>NormalOperationState!E9</f>
         <v>V</v>
@@ -1842,7 +1758,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.090000000000014</v>
       </c>
       <c r="B41" t="s">
@@ -1864,9 +1780,7 @@
         <f>NormalOperationState!D10</f>
         <v>315</v>
       </c>
-      <c r="G41" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G41" s="3"/>
       <c r="H41" s="3" t="str">
         <f>NormalOperationState!E10</f>
         <v>V</v>
@@ -1874,7 +1788,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.100000000000016</v>
       </c>
       <c r="B42" t="s">
@@ -1896,9 +1810,7 @@
         <f>NormalOperationState!D11</f>
         <v>0</v>
       </c>
-      <c r="G42" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G42" s="3"/>
       <c r="H42" s="3" t="str">
         <f>NormalOperationState!E11</f>
         <v>V</v>
@@ -1906,7 +1818,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.110000000000017</v>
       </c>
       <c r="B43" t="s">
@@ -1928,9 +1840,7 @@
         <f>NormalOperationState!D12</f>
         <v>800</v>
       </c>
-      <c r="G43" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G43" s="3"/>
       <c r="H43" s="3" t="str">
         <f>NormalOperationState!E12</f>
         <v>V</v>
@@ -1938,7 +1848,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.120000000000019</v>
       </c>
       <c r="B44" t="s">
@@ -1960,9 +1870,7 @@
         <f>NormalOperationState!D13</f>
         <v>0</v>
       </c>
-      <c r="G44" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G44" s="3"/>
       <c r="H44" s="3" t="str">
         <f>NormalOperationState!E13</f>
         <v>V</v>
@@ -1970,7 +1878,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.13000000000002</v>
       </c>
       <c r="B45" t="s">
@@ -1992,9 +1900,7 @@
         <f>NormalOperationState!D14</f>
         <v>24</v>
       </c>
-      <c r="G45" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G45" s="3"/>
       <c r="H45" s="3" t="str">
         <f>NormalOperationState!E14</f>
         <v>V</v>
@@ -2002,7 +1908,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>17.140000000000022</v>
       </c>
       <c r="B46" t="s">
@@ -2024,9 +1930,7 @@
         <f>NormalOperationState!D15</f>
         <v>0</v>
       </c>
-      <c r="G46" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G46" s="3"/>
       <c r="H46" s="3" t="str">
         <f>NormalOperationState!E15</f>
         <v>A</v>
@@ -2055,9 +1959,7 @@
         <f>SPMState!D2</f>
         <v>0</v>
       </c>
-      <c r="G47" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G47" s="3"/>
       <c r="H47" s="3" t="str">
         <f>SPMState!E2</f>
         <v>V</v>
@@ -2087,9 +1989,7 @@
         <f>SPMState!D3</f>
         <v>24</v>
       </c>
-      <c r="G48" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G48" s="3"/>
       <c r="H48" s="3" t="str">
         <f>SPMState!E3</f>
         <v>V</v>
@@ -2097,7 +1997,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <f t="shared" ref="A49:A61" si="6">A48+0.01</f>
+        <f t="shared" ref="A49:A61" si="5">A48+0.01</f>
         <v>18.030000000000005</v>
       </c>
       <c r="B49" t="s">
@@ -2119,9 +2019,7 @@
         <f>SPMState!D4</f>
         <v>0</v>
       </c>
-      <c r="G49" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G49" s="3"/>
       <c r="H49" s="3" t="str">
         <f>SPMState!E4</f>
         <v>V</v>
@@ -2129,7 +2027,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.040000000000006</v>
       </c>
       <c r="B50" t="s">
@@ -2151,9 +2049,7 @@
         <f>SPMState!D5</f>
         <v>24</v>
       </c>
-      <c r="G50" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G50" s="3"/>
       <c r="H50" s="3" t="str">
         <f>SPMState!E5</f>
         <v>V</v>
@@ -2161,7 +2057,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.050000000000008</v>
       </c>
       <c r="B51" t="s">
@@ -2183,9 +2079,7 @@
         <f>SPMState!D6</f>
         <v>5</v>
       </c>
-      <c r="G51" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G51" s="3"/>
       <c r="H51" s="3" t="str">
         <f>SPMState!E6</f>
         <v>V</v>
@@ -2193,7 +2087,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.060000000000009</v>
       </c>
       <c r="B52" t="s">
@@ -2215,9 +2109,7 @@
         <f>SPMState!D7</f>
         <v>0</v>
       </c>
-      <c r="G52" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G52" s="3"/>
       <c r="H52" s="3" t="str">
         <f>SPMState!E7</f>
         <v>V</v>
@@ -2225,7 +2117,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.070000000000011</v>
       </c>
       <c r="B53" t="s">
@@ -2247,9 +2139,7 @@
         <f>SPMState!D8</f>
         <v>5</v>
       </c>
-      <c r="G53" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G53" s="3"/>
       <c r="H53" s="3" t="str">
         <f>SPMState!E8</f>
         <v>V</v>
@@ -2257,7 +2147,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.080000000000013</v>
       </c>
       <c r="B54" t="s">
@@ -2279,9 +2169,7 @@
         <f>SPMState!D9</f>
         <v>0</v>
       </c>
-      <c r="G54" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G54" s="3"/>
       <c r="H54" s="3" t="str">
         <f>SPMState!E9</f>
         <v>V</v>
@@ -2289,7 +2177,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.090000000000014</v>
       </c>
       <c r="B55" t="s">
@@ -2311,9 +2199,7 @@
         <f>SPMState!D10</f>
         <v>240</v>
       </c>
-      <c r="G55" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G55" s="3"/>
       <c r="H55" s="3" t="str">
         <f>SPMState!E10</f>
         <v>V</v>
@@ -2321,7 +2207,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.100000000000016</v>
       </c>
       <c r="B56" t="s">
@@ -2343,9 +2229,7 @@
         <f>SPMState!D11</f>
         <v>240</v>
       </c>
-      <c r="G56" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G56" s="3"/>
       <c r="H56" s="3" t="str">
         <f>SPMState!E11</f>
         <v>V</v>
@@ -2353,7 +2237,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.110000000000017</v>
       </c>
       <c r="B57" t="s">
@@ -2375,9 +2259,7 @@
         <f>SPMState!D12</f>
         <v>800</v>
       </c>
-      <c r="G57" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G57" s="3"/>
       <c r="H57" s="3" t="str">
         <f>SPMState!E12</f>
         <v>V</v>
@@ -2385,7 +2267,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.120000000000019</v>
       </c>
       <c r="B58" t="s">
@@ -2407,9 +2289,7 @@
         <f>SPMState!D13</f>
         <v>16</v>
       </c>
-      <c r="G58" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G58" s="3"/>
       <c r="H58" s="3" t="str">
         <f>SPMState!E13</f>
         <v>V</v>
@@ -2417,7 +2297,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.13000000000002</v>
       </c>
       <c r="B59" t="s">
@@ -2439,9 +2319,7 @@
         <f>SPMState!D14</f>
         <v>24</v>
       </c>
-      <c r="G59" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G59" s="3"/>
       <c r="H59" s="3" t="str">
         <f>SPMState!E14</f>
         <v>V</v>
@@ -2449,7 +2327,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.140000000000022</v>
       </c>
       <c r="B60" t="s">
@@ -2471,9 +2349,7 @@
         <f>SPMState!D15</f>
         <v>0</v>
       </c>
-      <c r="G60" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G60" s="3"/>
       <c r="H60" s="3" t="str">
         <f>SPMState!E15</f>
         <v>A</v>
@@ -2481,7 +2357,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>18.150000000000023</v>
       </c>
       <c r="B61" t="s">
@@ -2503,9 +2379,7 @@
         <f>SPMState!D16</f>
         <v>95</v>
       </c>
-      <c r="G61" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G61" s="3"/>
       <c r="H61" s="3" t="str">
         <f>SPMState!E16</f>
         <v>%</v>
@@ -2534,9 +2408,7 @@
         <f>NoPowerState!D2</f>
         <v>0</v>
       </c>
-      <c r="G62" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G62" s="3"/>
       <c r="H62" s="3" t="str">
         <f>NoPowerState!E2</f>
         <v>V</v>
@@ -2566,9 +2438,7 @@
         <f>NoPowerState!D3</f>
         <v>0</v>
       </c>
-      <c r="G63" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G63" s="3"/>
       <c r="H63" s="3" t="str">
         <f>NoPowerState!E3</f>
         <v>V</v>
@@ -2576,7 +2446,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <f t="shared" ref="A64:A75" si="7">A63+0.01</f>
+        <f t="shared" ref="A64:A75" si="6">A63+0.01</f>
         <v>19.030000000000005</v>
       </c>
       <c r="B64" t="s">
@@ -2598,9 +2468,7 @@
         <f>NoPowerState!D4</f>
         <v>0</v>
       </c>
-      <c r="G64" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G64" s="3"/>
       <c r="H64" s="3" t="str">
         <f>NoPowerState!E4</f>
         <v>V</v>
@@ -2608,7 +2476,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.040000000000006</v>
       </c>
       <c r="B65" t="s">
@@ -2630,9 +2498,7 @@
         <f>NoPowerState!D5</f>
         <v>0</v>
       </c>
-      <c r="G65" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G65" s="3"/>
       <c r="H65" s="3" t="str">
         <f>NoPowerState!E5</f>
         <v>V</v>
@@ -2640,7 +2506,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.050000000000008</v>
       </c>
       <c r="B66" t="s">
@@ -2662,9 +2528,7 @@
         <f>NoPowerState!D6</f>
         <v>0</v>
       </c>
-      <c r="G66" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G66" s="3"/>
       <c r="H66" s="3" t="str">
         <f>NoPowerState!E6</f>
         <v>V</v>
@@ -2672,7 +2536,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.060000000000009</v>
       </c>
       <c r="B67" t="s">
@@ -2694,9 +2558,7 @@
         <f>NoPowerState!D7</f>
         <v>0</v>
       </c>
-      <c r="G67" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G67" s="3"/>
       <c r="H67" s="3" t="str">
         <f>NoPowerState!E7</f>
         <v>V</v>
@@ -2704,7 +2566,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.070000000000011</v>
       </c>
       <c r="B68" t="s">
@@ -2726,9 +2588,7 @@
         <f>NoPowerState!D8</f>
         <v>0</v>
       </c>
-      <c r="G68" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G68" s="3"/>
       <c r="H68" s="3" t="str">
         <f>NoPowerState!E8</f>
         <v>V</v>
@@ -2736,7 +2596,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.080000000000013</v>
       </c>
       <c r="B69" t="s">
@@ -2758,9 +2618,7 @@
         <f>NoPowerState!D9</f>
         <v>0</v>
       </c>
-      <c r="G69" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G69" s="3"/>
       <c r="H69" s="3" t="str">
         <f>NoPowerState!E9</f>
         <v>V</v>
@@ -2768,7 +2626,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.090000000000014</v>
       </c>
       <c r="B70" t="s">
@@ -2790,9 +2648,7 @@
         <f>NoPowerState!D10</f>
         <v>0</v>
       </c>
-      <c r="G70" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G70" s="3"/>
       <c r="H70" s="3" t="str">
         <f>NoPowerState!E10</f>
         <v>V</v>
@@ -2800,7 +2656,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.100000000000016</v>
       </c>
       <c r="B71" t="s">
@@ -2822,9 +2678,7 @@
         <f>NoPowerState!D11</f>
         <v>0</v>
       </c>
-      <c r="G71" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G71" s="3"/>
       <c r="H71" s="3" t="str">
         <f>NoPowerState!E11</f>
         <v>V</v>
@@ -2832,7 +2686,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.110000000000017</v>
       </c>
       <c r="B72" t="s">
@@ -2854,9 +2708,7 @@
         <f>NoPowerState!D12</f>
         <v>0</v>
       </c>
-      <c r="G72" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G72" s="3"/>
       <c r="H72" s="3" t="str">
         <f>NoPowerState!E12</f>
         <v>V</v>
@@ -2864,7 +2716,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.120000000000019</v>
       </c>
       <c r="B73" t="s">
@@ -2886,9 +2738,7 @@
         <f>NoPowerState!D13</f>
         <v>0</v>
       </c>
-      <c r="G73" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G73" s="3"/>
       <c r="H73" s="3" t="str">
         <f>NoPowerState!E13</f>
         <v>V</v>
@@ -2896,7 +2746,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.13000000000002</v>
       </c>
       <c r="B74" t="s">
@@ -2918,9 +2768,7 @@
         <f>NoPowerState!D14</f>
         <v>0</v>
       </c>
-      <c r="G74" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G74" s="3"/>
       <c r="H74" s="3" t="str">
         <f>NoPowerState!E14</f>
         <v>V</v>
@@ -2928,7 +2776,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>19.140000000000022</v>
       </c>
       <c r="B75" t="s">
@@ -2950,9 +2798,7 @@
         <f>NoPowerState!D15</f>
         <v>0</v>
       </c>
-      <c r="G75" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G75" s="3"/>
       <c r="H75" s="3" t="str">
         <f>NoPowerState!E15</f>
         <v>A</v>
@@ -2981,9 +2827,7 @@
         <f>BootstrapState!D2</f>
         <v>20</v>
       </c>
-      <c r="G76" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G76" s="3"/>
       <c r="H76" s="3" t="str">
         <f>BootstrapState!E2</f>
         <v>dv/dt</v>
@@ -3013,9 +2857,7 @@
         <f>BootstrapState!D3</f>
         <v>20</v>
       </c>
-      <c r="G77" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G77" s="3"/>
       <c r="H77" s="3" t="str">
         <f>BootstrapState!E3</f>
         <v>dv/dt</v>
@@ -3023,7 +2865,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f t="shared" ref="A78:A80" si="8">A77+0.01</f>
+        <f t="shared" ref="A78:A80" si="7">A77+0.01</f>
         <v>20.030000000000005</v>
       </c>
       <c r="B78" t="s">
@@ -3045,9 +2887,7 @@
         <f>BootstrapState!D4</f>
         <v>290</v>
       </c>
-      <c r="G78" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G78" s="3"/>
       <c r="H78" s="3" t="str">
         <f>BootstrapState!E4</f>
         <v>V</v>
@@ -3055,7 +2895,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>20.040000000000006</v>
       </c>
       <c r="B79" t="s">
@@ -3077,9 +2917,7 @@
         <f>BootstrapState!D5</f>
         <v>16</v>
       </c>
-      <c r="G79" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G79" s="3"/>
       <c r="H79" s="3" t="str">
         <f>BootstrapState!E5</f>
         <v>V</v>
@@ -3087,7 +2925,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>20.050000000000008</v>
       </c>
       <c r="B80" t="s">
@@ -3109,9 +2947,7 @@
         <f>BootstrapState!D6</f>
         <v>24</v>
       </c>
-      <c r="G80" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G80" s="3"/>
       <c r="H80" s="3" t="str">
         <f>BootstrapState!E6</f>
         <v>V</v>
@@ -3140,9 +2976,7 @@
         <f>SPMState!D2</f>
         <v>0</v>
       </c>
-      <c r="G81" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G81" s="3"/>
       <c r="H81" s="3" t="str">
         <f>SPMState!E2</f>
         <v>V</v>
@@ -3172,9 +3006,7 @@
         <f>SPMState!D3</f>
         <v>24</v>
       </c>
-      <c r="G82" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G82" s="3"/>
       <c r="H82" s="3" t="str">
         <f>SPMState!E3</f>
         <v>V</v>
@@ -3182,7 +3014,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" ref="A83:A95" si="9">A82+0.01</f>
+        <f t="shared" ref="A83:A95" si="8">A82+0.01</f>
         <v>21.030000000000005</v>
       </c>
       <c r="B83" t="s">
@@ -3204,9 +3036,7 @@
         <f>SPMState!D4</f>
         <v>0</v>
       </c>
-      <c r="G83" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G83" s="3"/>
       <c r="H83" s="3" t="str">
         <f>SPMState!E4</f>
         <v>V</v>
@@ -3214,7 +3044,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.040000000000006</v>
       </c>
       <c r="B84" t="s">
@@ -3236,9 +3066,7 @@
         <f>SPMState!D5</f>
         <v>24</v>
       </c>
-      <c r="G84" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G84" s="3"/>
       <c r="H84" s="3" t="str">
         <f>SPMState!E5</f>
         <v>V</v>
@@ -3246,7 +3074,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.050000000000008</v>
       </c>
       <c r="B85" t="s">
@@ -3268,9 +3096,7 @@
         <f>SPMState!D6</f>
         <v>5</v>
       </c>
-      <c r="G85" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G85" s="3"/>
       <c r="H85" s="3" t="str">
         <f>SPMState!E6</f>
         <v>V</v>
@@ -3278,7 +3104,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.060000000000009</v>
       </c>
       <c r="B86" t="s">
@@ -3300,9 +3126,7 @@
         <f>SPMState!D7</f>
         <v>0</v>
       </c>
-      <c r="G86" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G86" s="3"/>
       <c r="H86" s="3" t="str">
         <f>SPMState!E7</f>
         <v>V</v>
@@ -3310,7 +3134,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.070000000000011</v>
       </c>
       <c r="B87" t="s">
@@ -3332,9 +3156,7 @@
         <f>SPMState!D8</f>
         <v>5</v>
       </c>
-      <c r="G87" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G87" s="3"/>
       <c r="H87" s="3" t="str">
         <f>SPMState!E8</f>
         <v>V</v>
@@ -3342,7 +3164,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.080000000000013</v>
       </c>
       <c r="B88" t="s">
@@ -3364,9 +3186,7 @@
         <f>SPMState!D9</f>
         <v>0</v>
       </c>
-      <c r="G88" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G88" s="3"/>
       <c r="H88" s="3" t="str">
         <f>SPMState!E9</f>
         <v>V</v>
@@ -3374,7 +3194,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.090000000000014</v>
       </c>
       <c r="B89" t="s">
@@ -3396,9 +3216,7 @@
         <f>SPMState!D10</f>
         <v>240</v>
       </c>
-      <c r="G89" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G89" s="3"/>
       <c r="H89" s="3" t="str">
         <f>SPMState!E10</f>
         <v>V</v>
@@ -3406,7 +3224,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.100000000000016</v>
       </c>
       <c r="B90" t="s">
@@ -3428,9 +3246,7 @@
         <f>SPMState!D11</f>
         <v>240</v>
       </c>
-      <c r="G90" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G90" s="3"/>
       <c r="H90" s="3" t="str">
         <f>SPMState!E11</f>
         <v>V</v>
@@ -3438,7 +3254,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.110000000000017</v>
       </c>
       <c r="B91" t="s">
@@ -3460,9 +3276,7 @@
         <f>SPMState!D12</f>
         <v>800</v>
       </c>
-      <c r="G91" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G91" s="3"/>
       <c r="H91" s="3" t="str">
         <f>SPMState!E12</f>
         <v>V</v>
@@ -3470,7 +3284,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.120000000000019</v>
       </c>
       <c r="B92" t="s">
@@ -3492,9 +3306,7 @@
         <f>SPMState!D13</f>
         <v>16</v>
       </c>
-      <c r="G92" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G92" s="3"/>
       <c r="H92" s="3" t="str">
         <f>SPMState!E13</f>
         <v>V</v>
@@ -3502,7 +3314,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.13000000000002</v>
       </c>
       <c r="B93" t="s">
@@ -3524,9 +3336,7 @@
         <f>SPMState!D14</f>
         <v>24</v>
       </c>
-      <c r="G93" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G93" s="3"/>
       <c r="H93" s="3" t="str">
         <f>SPMState!E14</f>
         <v>V</v>
@@ -3534,7 +3344,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.140000000000022</v>
       </c>
       <c r="B94" t="s">
@@ -3556,9 +3366,7 @@
         <f>SPMState!D15</f>
         <v>0</v>
       </c>
-      <c r="G94" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G94" s="3"/>
       <c r="H94" s="3" t="str">
         <f>SPMState!E15</f>
         <v>A</v>
@@ -3566,7 +3374,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>21.150000000000023</v>
       </c>
       <c r="B95" t="s">
@@ -3588,9 +3396,7 @@
         <f>SPMState!D16</f>
         <v>95</v>
       </c>
-      <c r="G95" s="3">
-        <v>-999</v>
-      </c>
+      <c r="G95" s="3"/>
       <c r="H95" s="3" t="str">
         <f>SPMState!E16</f>
         <v>%</v>

</xml_diff>

<commit_message>
Tester.py -> setting hv and lv PS to 0,0 as a safety precaution during power down.  Updated Template with calculated Temp values in degC
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98DCA6A9-A019-4DB4-8400-0AB496F84914}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B52048-F4EA-4135-A77E-E67A1E57AD44}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1455" windowWidth="21600" windowHeight="11850" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="3096" yWindow="420" windowWidth="16668" windowHeight="10788" firstSheet="1" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="67">
   <si>
     <t>TEST #</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Threshold8</t>
+  </si>
+  <si>
+    <t>degC</t>
   </si>
 </sst>
 </file>
@@ -598,21 +601,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10:E15"/>
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -670,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>1+A2</f>
         <v>2</v>
@@ -697,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="2">1+A3</f>
         <v>3</v>
@@ -724,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -751,7 +754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -778,7 +781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -805,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -832,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -859,7 +862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -884,7 +887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -909,7 +912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -934,7 +937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -959,7 +962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -984,7 +987,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1009,7 +1012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15.01</v>
       </c>
@@ -1038,7 +1041,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f>A16+0.01</f>
         <v>15.02</v>
@@ -1068,7 +1071,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <f t="shared" ref="A18:A29" si="3">A17+0.01</f>
         <v>15.03</v>
@@ -1098,7 +1101,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>15.04</v>
@@ -1128,7 +1131,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>15.049999999999999</v>
@@ -1158,7 +1161,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>15.059999999999999</v>
@@ -1172,11 +1175,11 @@
       </c>
       <c r="D21" s="3">
         <f>NoPowerState!B7</f>
-        <v>-0.5</v>
+        <v>200</v>
       </c>
       <c r="E21" s="3">
         <f>NoPowerState!C7</f>
-        <v>0.5</v>
+        <v>210</v>
       </c>
       <c r="F21" s="3">
         <f>NoPowerState!D7</f>
@@ -1185,10 +1188,10 @@
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="str">
         <f>NoPowerState!E7</f>
-        <v>V</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>degC</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>15.069999999999999</v>
@@ -1218,7 +1221,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>15.079999999999998</v>
@@ -1248,7 +1251,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>15.089999999999998</v>
@@ -1278,7 +1281,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>15.099999999999998</v>
@@ -1308,7 +1311,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <f t="shared" si="3"/>
         <v>15.109999999999998</v>
@@ -1338,7 +1341,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <f>A26+0.01</f>
         <v>15.119999999999997</v>
@@ -1368,7 +1371,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>15.129999999999997</v>
@@ -1398,7 +1401,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>15.139999999999997</v>
@@ -1428,7 +1431,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>16.010000000000002</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <f>A30+0.01</f>
         <v>16.020000000000003</v>
@@ -1487,7 +1490,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <f>A31+0.01</f>
         <v>16.030000000000005</v>
@@ -1517,7 +1520,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>17.010000000000002</v>
       </c>
@@ -1546,7 +1549,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <f>A33+0.01</f>
         <v>17.020000000000003</v>
@@ -1576,7 +1579,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <f t="shared" ref="A35:A46" si="4">A34+0.01</f>
         <v>17.030000000000005</v>
@@ -1606,7 +1609,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <f t="shared" si="4"/>
         <v>17.040000000000006</v>
@@ -1636,7 +1639,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <f t="shared" si="4"/>
         <v>17.050000000000008</v>
@@ -1666,7 +1669,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <f t="shared" si="4"/>
         <v>17.060000000000009</v>
@@ -1680,11 +1683,11 @@
       </c>
       <c r="D38" s="3">
         <f>NormalOperationState!B7</f>
-        <v>-0.5</v>
+        <v>23.2</v>
       </c>
       <c r="E38" s="3">
         <f>NormalOperationState!C7</f>
-        <v>0.5</v>
+        <v>26.8</v>
       </c>
       <c r="F38" s="3">
         <f>NormalOperationState!D7</f>
@@ -1693,10 +1696,10 @@
       <c r="G38" s="3"/>
       <c r="H38" s="3" t="str">
         <f>NormalOperationState!E7</f>
-        <v>V</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>degC</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <f t="shared" si="4"/>
         <v>17.070000000000011</v>
@@ -1726,7 +1729,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <f t="shared" si="4"/>
         <v>17.080000000000013</v>
@@ -1756,7 +1759,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <f t="shared" si="4"/>
         <v>17.090000000000014</v>
@@ -1786,7 +1789,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <f t="shared" si="4"/>
         <v>17.100000000000016</v>
@@ -1816,7 +1819,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <f t="shared" si="4"/>
         <v>17.110000000000017</v>
@@ -1846,7 +1849,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <f t="shared" si="4"/>
         <v>17.120000000000019</v>
@@ -1876,7 +1879,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <f t="shared" si="4"/>
         <v>17.13000000000002</v>
@@ -1906,7 +1909,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <f t="shared" si="4"/>
         <v>17.140000000000022</v>
@@ -1936,7 +1939,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>18.010000000000002</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <f>A47+0.01</f>
         <v>18.020000000000003</v>
@@ -1995,7 +1998,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <f t="shared" ref="A49:A61" si="5">A48+0.01</f>
         <v>18.030000000000005</v>
@@ -2025,7 +2028,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <f t="shared" si="5"/>
         <v>18.040000000000006</v>
@@ -2055,7 +2058,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <f t="shared" si="5"/>
         <v>18.050000000000008</v>
@@ -2085,7 +2088,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <f t="shared" si="5"/>
         <v>18.060000000000009</v>
@@ -2112,10 +2115,10 @@
       <c r="G52" s="3"/>
       <c r="H52" s="3" t="str">
         <f>SPMState!E7</f>
-        <v>V</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+        <v>degC</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <f t="shared" si="5"/>
         <v>18.070000000000011</v>
@@ -2145,7 +2148,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <f t="shared" si="5"/>
         <v>18.080000000000013</v>
@@ -2175,7 +2178,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <f t="shared" si="5"/>
         <v>18.090000000000014</v>
@@ -2205,7 +2208,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <f t="shared" si="5"/>
         <v>18.100000000000016</v>
@@ -2235,7 +2238,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <f t="shared" si="5"/>
         <v>18.110000000000017</v>
@@ -2265,7 +2268,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <f t="shared" si="5"/>
         <v>18.120000000000019</v>
@@ -2295,7 +2298,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <f t="shared" si="5"/>
         <v>18.13000000000002</v>
@@ -2325,7 +2328,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <f t="shared" si="5"/>
         <v>18.140000000000022</v>
@@ -2355,7 +2358,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <f t="shared" si="5"/>
         <v>18.150000000000023</v>
@@ -2385,7 +2388,7 @@
         <v>%</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>19.010000000000002</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <f>A62+0.01</f>
         <v>19.020000000000003</v>
@@ -2444,7 +2447,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <f t="shared" ref="A64:A75" si="6">A63+0.01</f>
         <v>19.030000000000005</v>
@@ -2474,7 +2477,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <f t="shared" si="6"/>
         <v>19.040000000000006</v>
@@ -2504,7 +2507,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <f t="shared" si="6"/>
         <v>19.050000000000008</v>
@@ -2534,7 +2537,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <f t="shared" si="6"/>
         <v>19.060000000000009</v>
@@ -2548,11 +2551,11 @@
       </c>
       <c r="D67" s="3">
         <f>NoPowerState!B7</f>
-        <v>-0.5</v>
+        <v>200</v>
       </c>
       <c r="E67" s="3">
         <f>NoPowerState!C7</f>
-        <v>0.5</v>
+        <v>210</v>
       </c>
       <c r="F67" s="3">
         <f>NoPowerState!D7</f>
@@ -2561,10 +2564,10 @@
       <c r="G67" s="3"/>
       <c r="H67" s="3" t="str">
         <f>NoPowerState!E7</f>
-        <v>V</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>degC</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <f t="shared" si="6"/>
         <v>19.070000000000011</v>
@@ -2594,7 +2597,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <f t="shared" si="6"/>
         <v>19.080000000000013</v>
@@ -2624,7 +2627,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <f t="shared" si="6"/>
         <v>19.090000000000014</v>
@@ -2654,7 +2657,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <f t="shared" si="6"/>
         <v>19.100000000000016</v>
@@ -2684,7 +2687,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <f t="shared" si="6"/>
         <v>19.110000000000017</v>
@@ -2714,7 +2717,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <f t="shared" si="6"/>
         <v>19.120000000000019</v>
@@ -2744,7 +2747,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <f t="shared" si="6"/>
         <v>19.13000000000002</v>
@@ -2774,7 +2777,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <f t="shared" si="6"/>
         <v>19.140000000000022</v>
@@ -2804,7 +2807,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>20.010000000000002</v>
       </c>
@@ -2833,7 +2836,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <f>A76+0.01</f>
         <v>20.020000000000003</v>
@@ -2863,7 +2866,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <f t="shared" ref="A78:A80" si="7">A77+0.01</f>
         <v>20.030000000000005</v>
@@ -2893,7 +2896,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <f t="shared" si="7"/>
         <v>20.040000000000006</v>
@@ -2923,7 +2926,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <f t="shared" si="7"/>
         <v>20.050000000000008</v>
@@ -2953,7 +2956,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>21.01</v>
       </c>
@@ -2982,7 +2985,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <f>A81+0.01</f>
         <v>21.020000000000003</v>
@@ -3012,7 +3015,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <f t="shared" ref="A83:A95" si="8">A82+0.01</f>
         <v>21.030000000000005</v>
@@ -3042,7 +3045,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <f t="shared" si="8"/>
         <v>21.040000000000006</v>
@@ -3072,7 +3075,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <f t="shared" si="8"/>
         <v>21.050000000000008</v>
@@ -3102,7 +3105,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <f t="shared" si="8"/>
         <v>21.060000000000009</v>
@@ -3129,10 +3132,10 @@
       <c r="G86" s="3"/>
       <c r="H86" s="3" t="str">
         <f>SPMState!E7</f>
-        <v>V</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+        <v>degC</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <f t="shared" si="8"/>
         <v>21.070000000000011</v>
@@ -3162,7 +3165,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <f t="shared" si="8"/>
         <v>21.080000000000013</v>
@@ -3192,7 +3195,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <f t="shared" si="8"/>
         <v>21.090000000000014</v>
@@ -3222,7 +3225,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <f t="shared" si="8"/>
         <v>21.100000000000016</v>
@@ -3252,7 +3255,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <f t="shared" si="8"/>
         <v>21.110000000000017</v>
@@ -3282,7 +3285,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <f t="shared" si="8"/>
         <v>21.120000000000019</v>
@@ -3312,7 +3315,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <f t="shared" si="8"/>
         <v>21.13000000000002</v>
@@ -3342,7 +3345,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <f t="shared" si="8"/>
         <v>21.140000000000022</v>
@@ -3372,7 +3375,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <f t="shared" si="8"/>
         <v>21.150000000000023</v>
@@ -3412,16 +3415,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660F8094-D216-4D3A-9488-AF9A051CC77B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3438,7 +3441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3455,7 +3458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3472,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3489,7 +3492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3506,7 +3509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3523,24 +3526,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="3">
-        <v>-0.5</v>
+        <v>200</v>
       </c>
       <c r="C7" s="3">
-        <v>0.5</v>
+        <v>210</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3557,7 +3560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3574,7 +3577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3591,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3608,7 +3611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3625,7 +3628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3642,7 +3645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3659,7 +3662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3686,15 +3689,15 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3711,7 +3714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3728,7 +3731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3745,7 +3748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3762,7 +3765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3796,24 +3799,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
       <c r="B7" s="3">
-        <v>-0.5</v>
+        <v>23.2</v>
       </c>
       <c r="C7" s="3">
-        <v>0.5</v>
+        <v>26.8</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3830,7 +3833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3847,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3864,7 +3867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3881,7 +3884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3898,7 +3901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3915,7 +3918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3962,9 +3965,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -3998,7 +4001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4015,7 +4018,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4042,17 +4045,17 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4086,7 +4089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4103,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4120,7 +4123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4154,7 +4157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4168,10 +4171,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4188,7 +4191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4205,7 +4208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4222,7 +4225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4239,7 +4242,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4256,7 +4259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4273,7 +4276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4290,7 +4293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4307,7 +4310,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -4337,12 +4340,12 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4359,7 +4362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -4376,7 +4379,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4393,7 +4396,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4410,7 +4413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4427,7 +4430,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -4444,12 +4447,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4464,15 +4467,15 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -4486,7 +4489,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4500,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4514,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4528,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4542,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4556,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4564,13 +4567,13 @@
         <v>206</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>-75</v>
       </c>
       <c r="D7">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4584,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4598,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4612,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4626,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4640,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4654,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4668,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Updated temp on template2 to be 25degC, 29 degCprior was because the board was heated up too long, PwrTestIO updated with quicker discharge cap at 10V check Tester.py fixed input diode setup with closing RL5, applying 24V and turning off load. Tester.py fixed catch fail for diode checks and fixed false pass issue
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F81DEEE-DAD1-4EF4-AD57-D25724ADE4B1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F187165B-CBC3-47B5-96CE-CAEE0657CC88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5676" yWindow="864" windowWidth="16668" windowHeight="10788" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="14172" windowHeight="10788" firstSheet="3" activeTab="6" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="E28" s="3">
         <f>NoPowerState!C14</f>
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="F28" s="3">
         <f>NoPowerState!D14</f>
@@ -1504,15 +1504,15 @@
       </c>
       <c r="D32" s="3">
         <f>CapsChargingState!B4</f>
-        <v>23</v>
+        <v>23.8</v>
       </c>
       <c r="E32" s="3">
         <f>CapsChargingState!C4</f>
-        <v>25</v>
+        <v>26.2</v>
       </c>
       <c r="F32" s="3">
         <f>CapsChargingState!D4</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="str">
@@ -1683,15 +1683,15 @@
       </c>
       <c r="D38" s="3">
         <f>NormalOperationState!B7</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E38" s="3">
         <f>NormalOperationState!C7</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F38" s="3">
         <f>NormalOperationState!D7</f>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3" t="str">
@@ -2102,15 +2102,15 @@
       </c>
       <c r="D52" s="3">
         <f>SPMState!B7</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E52" s="3">
         <f>SPMState!C7</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F52" s="3">
         <f>SPMState!D7</f>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3" t="str">
@@ -2765,7 +2765,7 @@
       </c>
       <c r="E74" s="3">
         <f>NoPowerState!C14</f>
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="F74" s="3">
         <f>NoPowerState!D14</f>
@@ -3119,15 +3119,15 @@
       </c>
       <c r="D86" s="3">
         <f>SPMState!B7</f>
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E86" s="3">
         <f>SPMState!C7</f>
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F86" s="3">
         <f>SPMState!D7</f>
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3" t="str">
@@ -3416,7 +3416,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3653,7 +3653,7 @@
         <v>-0.5</v>
       </c>
       <c r="C14" s="3">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -3689,7 +3689,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="B7:D7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3804,13 +3804,13 @@
         <v>41</v>
       </c>
       <c r="B7" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>66</v>
@@ -3962,7 +3962,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4023,13 +4023,13 @@
         <v>47</v>
       </c>
       <c r="B4" s="3">
-        <v>23</v>
+        <v>23.8</v>
       </c>
       <c r="C4" s="3">
+        <v>26.2</v>
+      </c>
+      <c r="D4" s="3">
         <v>25</v>
-      </c>
-      <c r="D4" s="3">
-        <v>24</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -4045,7 +4045,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4162,13 +4162,13 @@
         <v>41</v>
       </c>
       <c r="B7" s="3">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D7" s="3">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>66</v>
@@ -4466,7 +4466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CEAD3C-E293-403D-9957-624DD4ECBBD6}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
I think all we have left is measurement error issues!
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F187165B-CBC3-47B5-96CE-CAEE0657CC88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB90140B-BCFE-4236-BC11-F0042F183C88}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="14172" windowHeight="10788" firstSheet="3" activeTab="6" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -602,20 +602,20 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O82" sqref="O82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,7 +647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -673,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
         <v>2</v>
@@ -700,7 +700,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="2">1+A3</f>
         <v>3</v>
@@ -727,7 +727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -754,7 +754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -781,7 +781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -808,7 +808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -835,7 +835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -862,7 +862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -887,7 +887,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -912,7 +912,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -937,7 +937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -962,7 +962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -987,7 +987,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1012,7 +1012,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15.01</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>A16+0.01</f>
         <v>15.02</v>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E17" s="3">
         <f>NoPowerState!C3</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F17" s="3">
         <f>NoPowerState!D3</f>
@@ -1071,7 +1071,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" ref="A18:A29" si="3">A17+0.01</f>
         <v>15.03</v>
@@ -1101,7 +1101,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="3"/>
         <v>15.04</v>
@@ -1131,7 +1131,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="3"/>
         <v>15.049999999999999</v>
@@ -1161,7 +1161,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="3"/>
         <v>15.059999999999999</v>
@@ -1191,7 +1191,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="3"/>
         <v>15.069999999999999</v>
@@ -1221,7 +1221,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="3"/>
         <v>15.079999999999998</v>
@@ -1251,7 +1251,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="3"/>
         <v>15.089999999999998</v>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="E24" s="3">
         <f>NoPowerState!C10</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="F24" s="3">
         <f>NoPowerState!D10</f>
@@ -1281,7 +1281,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="3"/>
         <v>15.099999999999998</v>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="E25" s="3">
         <f>NoPowerState!C11</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F25" s="3">
         <f>NoPowerState!D11</f>
@@ -1311,7 +1311,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="3"/>
         <v>15.109999999999998</v>
@@ -1329,7 +1329,7 @@
       </c>
       <c r="E26" s="3">
         <f>NoPowerState!C12</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F26" s="3">
         <f>NoPowerState!D12</f>
@@ -1341,7 +1341,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>A26+0.01</f>
         <v>15.119999999999997</v>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="E27" s="3">
         <f>NoPowerState!C13</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F27" s="3">
         <f>NoPowerState!D13</f>
@@ -1371,7 +1371,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="3"/>
         <v>15.129999999999997</v>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="E28" s="3">
         <f>NoPowerState!C14</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F28" s="3">
         <f>NoPowerState!D14</f>
@@ -1401,7 +1401,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="3"/>
         <v>15.139999999999997</v>
@@ -1431,7 +1431,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>16.010000000000002</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>A30+0.01</f>
         <v>16.020000000000003</v>
@@ -1490,7 +1490,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>A31+0.01</f>
         <v>16.030000000000005</v>
@@ -1520,7 +1520,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>17.010000000000002</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>A33+0.01</f>
         <v>17.020000000000003</v>
@@ -1579,7 +1579,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" ref="A35:A46" si="4">A34+0.01</f>
         <v>17.030000000000005</v>
@@ -1609,7 +1609,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="4"/>
         <v>17.040000000000006</v>
@@ -1639,7 +1639,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="4"/>
         <v>17.050000000000008</v>
@@ -1669,7 +1669,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="4"/>
         <v>17.060000000000009</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="E38" s="3">
         <f>NormalOperationState!C7</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F38" s="3">
         <f>NormalOperationState!D7</f>
@@ -1699,7 +1699,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="4"/>
         <v>17.070000000000011</v>
@@ -1729,7 +1729,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="4"/>
         <v>17.080000000000013</v>
@@ -1759,7 +1759,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="4"/>
         <v>17.090000000000014</v>
@@ -1789,7 +1789,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="4"/>
         <v>17.100000000000016</v>
@@ -1819,7 +1819,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="4"/>
         <v>17.110000000000017</v>
@@ -1849,7 +1849,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="4"/>
         <v>17.120000000000019</v>
@@ -1879,7 +1879,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="4"/>
         <v>17.13000000000002</v>
@@ -1909,7 +1909,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="4"/>
         <v>17.140000000000022</v>
@@ -1939,7 +1939,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18.010000000000002</v>
       </c>
@@ -1952,7 +1952,7 @@
       </c>
       <c r="D47" s="3">
         <f>SPMState!B2</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="E47" s="3">
         <f>SPMState!C2</f>
@@ -1968,7 +1968,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>A47+0.01</f>
         <v>18.020000000000003</v>
@@ -1998,7 +1998,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" ref="A49:A61" si="5">A48+0.01</f>
         <v>18.030000000000005</v>
@@ -2028,7 +2028,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="5"/>
         <v>18.040000000000006</v>
@@ -2058,7 +2058,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="5"/>
         <v>18.050000000000008</v>
@@ -2088,7 +2088,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="5"/>
         <v>18.060000000000009</v>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="E52" s="3">
         <f>SPMState!C7</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F52" s="3">
         <f>SPMState!D7</f>
@@ -2118,7 +2118,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="5"/>
         <v>18.070000000000011</v>
@@ -2148,7 +2148,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="5"/>
         <v>18.080000000000013</v>
@@ -2178,7 +2178,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="5"/>
         <v>18.090000000000014</v>
@@ -2208,7 +2208,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="5"/>
         <v>18.100000000000016</v>
@@ -2238,7 +2238,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="5"/>
         <v>18.110000000000017</v>
@@ -2252,7 +2252,7 @@
       </c>
       <c r="D57" s="3">
         <f>SPMState!B12</f>
-        <v>799</v>
+        <v>280</v>
       </c>
       <c r="E57" s="3">
         <f>SPMState!C12</f>
@@ -2268,7 +2268,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="5"/>
         <v>18.120000000000019</v>
@@ -2298,7 +2298,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="5"/>
         <v>18.13000000000002</v>
@@ -2328,7 +2328,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="5"/>
         <v>18.140000000000022</v>
@@ -2342,15 +2342,15 @@
       </c>
       <c r="D60" s="3">
         <f>SPMState!B15</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E60" s="3">
         <f>SPMState!C15</f>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F60" s="3">
         <f>SPMState!D15</f>
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3" t="str">
@@ -2358,7 +2358,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="5"/>
         <v>18.150000000000023</v>
@@ -2388,7 +2388,7 @@
         <v>%</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>19.010000000000002</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>A62+0.01</f>
         <v>19.020000000000003</v>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="E63" s="3">
         <f>NoPowerState!C3</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F63" s="3">
         <f>NoPowerState!D3</f>
@@ -2447,7 +2447,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" ref="A64:A75" si="6">A63+0.01</f>
         <v>19.030000000000005</v>
@@ -2477,7 +2477,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="6"/>
         <v>19.040000000000006</v>
@@ -2507,7 +2507,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="6"/>
         <v>19.050000000000008</v>
@@ -2537,7 +2537,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="6"/>
         <v>19.060000000000009</v>
@@ -2567,7 +2567,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="6"/>
         <v>19.070000000000011</v>
@@ -2597,7 +2597,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="6"/>
         <v>19.080000000000013</v>
@@ -2627,7 +2627,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="6"/>
         <v>19.090000000000014</v>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="E70" s="3">
         <f>NoPowerState!C10</f>
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="F70" s="3">
         <f>NoPowerState!D10</f>
@@ -2657,7 +2657,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="6"/>
         <v>19.100000000000016</v>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="E71" s="3">
         <f>NoPowerState!C11</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F71" s="3">
         <f>NoPowerState!D11</f>
@@ -2687,7 +2687,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="6"/>
         <v>19.110000000000017</v>
@@ -2705,7 +2705,7 @@
       </c>
       <c r="E72" s="3">
         <f>NoPowerState!C12</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F72" s="3">
         <f>NoPowerState!D12</f>
@@ -2717,7 +2717,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="6"/>
         <v>19.120000000000019</v>
@@ -2735,7 +2735,7 @@
       </c>
       <c r="E73" s="3">
         <f>NoPowerState!C13</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="F73" s="3">
         <f>NoPowerState!D13</f>
@@ -2747,7 +2747,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="6"/>
         <v>19.13000000000002</v>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="E74" s="3">
         <f>NoPowerState!C14</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F74" s="3">
         <f>NoPowerState!D14</f>
@@ -2777,7 +2777,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="6"/>
         <v>19.140000000000022</v>
@@ -2807,7 +2807,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20.010000000000002</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>A76+0.01</f>
         <v>20.020000000000003</v>
@@ -2866,7 +2866,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" ref="A78:A80" si="7">A77+0.01</f>
         <v>20.030000000000005</v>
@@ -2896,7 +2896,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="7"/>
         <v>20.040000000000006</v>
@@ -2926,7 +2926,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="7"/>
         <v>20.050000000000008</v>
@@ -2940,7 +2940,7 @@
       </c>
       <c r="D80" s="3">
         <f>BootstrapState!B6</f>
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E80" s="3">
         <f>BootstrapState!C6</f>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="F80" s="3">
         <f>BootstrapState!D6</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3" t="str">
@@ -2956,7 +2956,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>21.01</v>
       </c>
@@ -2969,7 +2969,7 @@
       </c>
       <c r="D81" s="3">
         <f>SPMState!B2</f>
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="E81" s="3">
         <f>SPMState!C2</f>
@@ -2985,7 +2985,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f>A81+0.01</f>
         <v>21.020000000000003</v>
@@ -3015,7 +3015,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" ref="A83:A95" si="8">A82+0.01</f>
         <v>21.030000000000005</v>
@@ -3045,7 +3045,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="8"/>
         <v>21.040000000000006</v>
@@ -3075,7 +3075,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="8"/>
         <v>21.050000000000008</v>
@@ -3105,7 +3105,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="8"/>
         <v>21.060000000000009</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="E86" s="3">
         <f>SPMState!C7</f>
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F86" s="3">
         <f>SPMState!D7</f>
@@ -3135,7 +3135,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="8"/>
         <v>21.070000000000011</v>
@@ -3165,7 +3165,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="8"/>
         <v>21.080000000000013</v>
@@ -3195,7 +3195,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="8"/>
         <v>21.090000000000014</v>
@@ -3225,7 +3225,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="8"/>
         <v>21.100000000000016</v>
@@ -3255,7 +3255,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="8"/>
         <v>21.110000000000017</v>
@@ -3269,7 +3269,7 @@
       </c>
       <c r="D91" s="3">
         <f>SPMState!B12</f>
-        <v>799</v>
+        <v>280</v>
       </c>
       <c r="E91" s="3">
         <f>SPMState!C12</f>
@@ -3285,7 +3285,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="8"/>
         <v>21.120000000000019</v>
@@ -3315,7 +3315,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="8"/>
         <v>21.13000000000002</v>
@@ -3345,7 +3345,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="8"/>
         <v>21.140000000000022</v>
@@ -3359,15 +3359,15 @@
       </c>
       <c r="D94" s="3">
         <f>SPMState!B15</f>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E94" s="3">
         <f>SPMState!C15</f>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="F94" s="3">
         <f>SPMState!D15</f>
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3" t="str">
@@ -3375,7 +3375,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="8"/>
         <v>21.150000000000023</v>
@@ -3415,16 +3415,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660F8094-D216-4D3A-9488-AF9A051CC77B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3458,7 +3458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>-0.5</v>
       </c>
       <c r="C3" s="3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
@@ -3475,7 +3475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>-0.5</v>
       </c>
       <c r="C10" s="3">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -3594,7 +3594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>-0.5</v>
       </c>
       <c r="C11" s="3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -3611,7 +3611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>-0.5</v>
       </c>
       <c r="C12" s="3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -3628,7 +3628,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>-0.5</v>
       </c>
       <c r="C13" s="3">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3">
         <v>0</v>
@@ -3645,7 +3645,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>-0.5</v>
       </c>
       <c r="C14" s="3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -3662,7 +3662,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3689,15 +3689,15 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3731,7 +3731,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3">
         <v>25</v>
@@ -3816,7 +3816,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3833,7 +3833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3867,7 +3867,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3965,9 +3965,9 @@
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4001,7 +4001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4018,7 +4018,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4045,17 +4045,17 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4072,12 +4072,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="3">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="C2" s="3">
         <v>0.5</v>
@@ -4089,7 +4089,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4140,7 +4140,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D7" s="3">
         <v>25</v>
@@ -4174,7 +4174,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4191,7 +4191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4242,12 +4242,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="3">
-        <v>799</v>
+        <v>280</v>
       </c>
       <c r="C12" s="3">
         <v>840</v>
@@ -4259,7 +4259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4293,24 +4293,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
       <c r="B15" s="3">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C15" s="3">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>0.73</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -4337,15 +4337,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4396,7 +4396,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4430,29 +4430,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="3">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3">
         <v>25</v>
       </c>
       <c r="D6" s="3">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4466,16 +4466,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CEAD3C-E293-403D-9957-624DD4ECBBD6}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4559,7 +4559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4587,7 +4587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4629,7 +4629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
Updated GUI to have AK label, HW Checker Save results, able to export save results into desktop/Test_Results folder as a .csv file, added HW Checker S/N text box and added DUT rev text box Updated Test Report Template for what we want to check on the HW checker
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED1FAE4-B7A3-4E75-9C51-4B300387F516}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3527C62-2D68-4783-B33B-881A4713869A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="21396" windowHeight="11352" activeTab="1" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="84">
   <si>
     <t>TEST #</t>
   </si>
@@ -239,6 +239,57 @@
   </si>
   <si>
     <t>degC</t>
+  </si>
+  <si>
+    <t>PSUA Check</t>
+  </si>
+  <si>
+    <t>PSUB Check</t>
+  </si>
+  <si>
+    <t>TP5B Check</t>
+  </si>
+  <si>
+    <t>TP1B Check</t>
+  </si>
+  <si>
+    <t>HVCAP Check</t>
+  </si>
+  <si>
+    <t>PSU_FLT Check</t>
+  </si>
+  <si>
+    <t>SPM Check</t>
+  </si>
+  <si>
+    <t>FLT_OUT Check</t>
+  </si>
+  <si>
+    <t>load1 Check</t>
+  </si>
+  <si>
+    <t>load2 Check</t>
+  </si>
+  <si>
+    <t>load3 Check</t>
+  </si>
+  <si>
+    <t>Load1</t>
+  </si>
+  <si>
+    <t>Load2</t>
+  </si>
+  <si>
+    <t>Load3</t>
+  </si>
+  <si>
+    <t>Ribbon1</t>
+  </si>
+  <si>
+    <t>Ribbon2</t>
+  </si>
+  <si>
+    <t>Ribbon3</t>
   </si>
 </sst>
 </file>
@@ -3416,7 +3467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{660F8094-D216-4D3A-9488-AF9A051CC77B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -4695,9 +4746,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3A8150-0F2A-4305-BFC4-9E49C077B26A}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4705,6 +4756,8 @@
     <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -4744,10 +4797,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <f>0.95*F2</f>
@@ -4771,10 +4824,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D9" si="0">0.95*F3</f>
@@ -4798,10 +4851,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
@@ -4825,10 +4878,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
@@ -4852,10 +4905,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
@@ -4879,10 +4932,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
@@ -4906,10 +4959,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
@@ -4933,10 +4986,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
@@ -4960,10 +5013,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -4976,7 +5029,7 @@
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -4985,10 +5038,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>82</v>
       </c>
       <c r="D11" s="3">
         <v>0</v>
@@ -5001,7 +5054,7 @@
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -5010,10 +5063,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>83</v>
       </c>
       <c r="D12" s="3">
         <v>0</v>
@@ -5026,83 +5079,32 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F13" s="3">
-        <v>0</v>
-      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="2"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0</v>
-      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="2"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0</v>
-      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="H15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated GUI interface colors, added HW checker run all/run none buttons updated pwr board hw checker items on template
updated pwr test gui so that it can properly save hw checker info
added selftester2 hw checker
increased timeout so that it will flag if goes past min limit
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3527C62-2D68-4783-B33B-881A4713869A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4DDA9-E4ED-4936-AE93-FFFFB147F9B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="4788" yWindow="288" windowWidth="16032" windowHeight="10800" firstSheet="4" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="HWCheck" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="145">
   <si>
     <t>TEST #</t>
   </si>
@@ -241,27 +242,12 @@
     <t>degC</t>
   </si>
   <si>
-    <t>PSUA Check</t>
-  </si>
-  <si>
-    <t>PSUB Check</t>
-  </si>
-  <si>
-    <t>TP5B Check</t>
-  </si>
-  <si>
     <t>TP1B Check</t>
   </si>
   <si>
     <t>HVCAP Check</t>
   </si>
   <si>
-    <t>PSU_FLT Check</t>
-  </si>
-  <si>
-    <t>SPM Check</t>
-  </si>
-  <si>
     <t>FLT_OUT Check</t>
   </si>
   <si>
@@ -290,6 +276,204 @@
   </si>
   <si>
     <t>Ribbon3</t>
+  </si>
+  <si>
+    <t>PSUA1</t>
+  </si>
+  <si>
+    <t>PSUA Check 5V</t>
+  </si>
+  <si>
+    <t>PSUA Check 25V</t>
+  </si>
+  <si>
+    <t>PSUA Check 15V</t>
+  </si>
+  <si>
+    <t>PSUA Check 20V</t>
+  </si>
+  <si>
+    <t>PSUA Check 10V</t>
+  </si>
+  <si>
+    <t>PSUA2</t>
+  </si>
+  <si>
+    <t>PSUA3</t>
+  </si>
+  <si>
+    <t>PSUA4</t>
+  </si>
+  <si>
+    <t>PSUA5</t>
+  </si>
+  <si>
+    <t>PSUB Check 5V</t>
+  </si>
+  <si>
+    <t>PSUB Check 15V</t>
+  </si>
+  <si>
+    <t>PSUB Check 25V</t>
+  </si>
+  <si>
+    <t>PSUB Check 20V</t>
+  </si>
+  <si>
+    <t>PSUB Check 10V</t>
+  </si>
+  <si>
+    <t>PSUB1</t>
+  </si>
+  <si>
+    <t>PSUB2</t>
+  </si>
+  <si>
+    <t>PSUB3</t>
+  </si>
+  <si>
+    <t>PSUB4</t>
+  </si>
+  <si>
+    <t>PSUB5</t>
+  </si>
+  <si>
+    <t>PSUC Check 5V</t>
+  </si>
+  <si>
+    <t>PSUC1</t>
+  </si>
+  <si>
+    <t>PSUC2</t>
+  </si>
+  <si>
+    <t>PSUC3</t>
+  </si>
+  <si>
+    <t>PSUC4</t>
+  </si>
+  <si>
+    <t>PSUC5</t>
+  </si>
+  <si>
+    <t>PSUC Check 15V</t>
+  </si>
+  <si>
+    <t>PSUC Check 25V</t>
+  </si>
+  <si>
+    <t>PSUC Check 20V</t>
+  </si>
+  <si>
+    <t>PSUC Check 10V</t>
+  </si>
+  <si>
+    <t>TP2B Check</t>
+  </si>
+  <si>
+    <t>TP5B1</t>
+  </si>
+  <si>
+    <t>TP5B2</t>
+  </si>
+  <si>
+    <t>TP5B3</t>
+  </si>
+  <si>
+    <t>TP5B4</t>
+  </si>
+  <si>
+    <t>TP5B5</t>
+  </si>
+  <si>
+    <t>TP6B Check</t>
+  </si>
+  <si>
+    <t>TP6B1</t>
+  </si>
+  <si>
+    <t>TP6B2</t>
+  </si>
+  <si>
+    <t>TP6B3</t>
+  </si>
+  <si>
+    <t>TP6B4</t>
+  </si>
+  <si>
+    <t>TP6B5</t>
+  </si>
+  <si>
+    <t>no load Check</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>Ribbon4</t>
+  </si>
+  <si>
+    <t>DS1 Check</t>
+  </si>
+  <si>
+    <t>DS2 Check</t>
+  </si>
+  <si>
+    <t>DS3 Check</t>
+  </si>
+  <si>
+    <t>DS4 Check</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>MOhm</t>
+  </si>
+  <si>
+    <t>TP5B Check 6V</t>
+  </si>
+  <si>
+    <t>TP5B Check 12V</t>
+  </si>
+  <si>
+    <t>TP5B Check 18V</t>
+  </si>
+  <si>
+    <t>TP5B Check 24V</t>
+  </si>
+  <si>
+    <t>TP5B Check 30V</t>
+  </si>
+  <si>
+    <t>PSU_FLT Buck OFF</t>
+  </si>
+  <si>
+    <t>PSU_FLT Buck ON</t>
+  </si>
+  <si>
+    <t>SPM OFF FB</t>
+  </si>
+  <si>
+    <t>TEMP OFF FB</t>
+  </si>
+  <si>
+    <t>SPM ON FB</t>
+  </si>
+  <si>
+    <t>TEMP ON FB</t>
+  </si>
+  <si>
+    <t>Ribbon5</t>
+  </si>
+  <si>
+    <t>Ribbon6</t>
+  </si>
+  <si>
+    <t>Ribbon7</t>
   </si>
 </sst>
 </file>
@@ -654,7 +838,7 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3468,7 +3652,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4519,7 +4703,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4661,7 +4845,7 @@
         <v>210</v>
       </c>
       <c r="C10">
-        <v>3.0041699999999998</v>
+        <v>2.998796</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4675,7 +4859,7 @@
         <v>211</v>
       </c>
       <c r="C11">
-        <v>3.0043790000000001</v>
+        <v>2.9995980000000002</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -4689,7 +4873,7 @@
         <v>212</v>
       </c>
       <c r="C12">
-        <v>3.0013649999999998</v>
+        <v>2.9991970000000001</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -4744,17 +4928,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3A8150-0F2A-4305-BFC4-9E49C077B26A}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
@@ -4794,24 +4980,24 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>1.01</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="D2" s="2">
-        <f>0.95*F2</f>
-        <v>19.170999999999999</v>
+        <f>0.98*F2</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E2" s="2">
-        <f>1.05*F2</f>
-        <v>21.189</v>
+        <f>1.02*F2</f>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F2" s="2">
-        <v>20.18</v>
+        <v>5</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
@@ -4820,25 +5006,24 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>1+A2</f>
-        <v>2</v>
+        <v>1.02</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D9" si="0">0.95*F3</f>
-        <v>19.170999999999999</v>
+        <f t="shared" ref="D3:D6" si="0">0.98*F3</f>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="1">1.05*F3</f>
-        <v>21.189</v>
+        <f t="shared" ref="E3:E16" si="1">1.02*F3</f>
+        <v>10.199999999999999</v>
       </c>
       <c r="F3" s="2">
-        <v>20.18</v>
+        <v>10</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
@@ -4847,25 +5032,24 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f t="shared" ref="A4:A15" si="2">1+A3</f>
-        <v>3</v>
+        <v>1.03</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>28.689999999999998</v>
+        <v>14.7</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="1"/>
-        <v>31.71</v>
+        <v>15.3</v>
       </c>
       <c r="F4" s="2">
-        <v>30.2</v>
+        <v>15</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
@@ -4874,25 +5058,24 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <v>1.04</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>28.689999999999998</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="1"/>
-        <v>31.71</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="F5" s="2">
-        <v>30.2</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
@@ -4901,25 +5084,24 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1.05</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>19.170999999999999</v>
+        <v>24.5</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>21.189</v>
+        <v>25.5</v>
       </c>
       <c r="F6" s="2">
-        <v>20.18</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
@@ -4928,25 +5110,24 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" si="0"/>
-        <v>19.170999999999999</v>
+        <f t="shared" ref="D7:D11" si="2">0.98*F7</f>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>21.189</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="F7" s="2">
-        <v>20.18</v>
+        <v>5</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
@@ -4955,25 +5136,24 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>2.02</v>
+      </c>
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="2">
-        <f t="shared" si="0"/>
-        <v>28.689999999999998</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>31.71</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F8" s="2">
-        <v>30.2</v>
+        <v>10</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
@@ -4982,25 +5162,24 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="B9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="2">
-        <f t="shared" si="0"/>
-        <v>28.689999999999998</v>
+        <v>14.7</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>31.71</v>
+        <v>15.3</v>
       </c>
       <c r="F9" s="2">
-        <v>30.2</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
@@ -5009,23 +5188,24 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>2.04</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F10" s="3">
-        <v>0</v>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
@@ -5034,23 +5214,24 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F11" s="3">
-        <v>0</v>
+        <v>24.5</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+      <c r="F11" s="2">
+        <v>25</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
@@ -5059,23 +5240,24 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <v>2.06</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1E-3</v>
-      </c>
-      <c r="F12" s="3">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12:D16" si="3">0.98*F12</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
@@ -5083,28 +5265,1116 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
       <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="A14">
+        <v>2.08</v>
+      </c>
+      <c r="B14" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="3"/>
+        <v>14.7</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>15.3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>15</v>
+      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="A15">
+        <v>2.09</v>
+      </c>
+      <c r="B15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="3"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>20.399999999999999</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20</v>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>2.1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="3"/>
+        <v>24.5</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>25.5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>25</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3.01</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" ref="D17:D45" si="4">0.95*F17</f>
+        <v>5.89</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" ref="E17:E45" si="5">1.05*F17</f>
+        <v>6.5100000000000007</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>3.02</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="4"/>
+        <v>11.685</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="5"/>
+        <v>12.915000000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>3.03</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" ref="D19:D21" si="6">0.95*F19</f>
+        <v>17.479999999999997</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" ref="E19:E21" si="7">1.05*F19</f>
+        <v>19.32</v>
+      </c>
+      <c r="F19" s="2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3.04</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="6"/>
+        <v>23.179999999999996</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="7"/>
+        <v>25.62</v>
+      </c>
+      <c r="F20" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>3.05</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" s="2">
+        <f t="shared" si="6"/>
+        <v>28.88</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="7"/>
+        <v>31.919999999999998</v>
+      </c>
+      <c r="F21" s="2">
+        <v>30.4</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>3.06</v>
+      </c>
+      <c r="B22" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" s="2">
+        <f t="shared" ref="D22" si="8">0.95*F22</f>
+        <v>0.95</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" ref="E22" si="9">1.05*F22</f>
+        <v>1.05</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>3.07</v>
+      </c>
+      <c r="B23" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="2">
+        <f t="shared" ref="D23:D36" si="10">0.95*F23</f>
+        <v>1.9</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" ref="E23:E36" si="11">1.05*F23</f>
+        <v>2.1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>2</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>3.08</v>
+      </c>
+      <c r="B24" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" s="2">
+        <f t="shared" si="10"/>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" si="11"/>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="F24" s="2">
+        <v>3</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>3.09</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D25" s="2">
+        <f t="shared" si="10"/>
+        <v>3.8</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="11"/>
+        <v>4.2</v>
+      </c>
+      <c r="F25" s="2">
+        <v>4</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3.1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="2">
+        <f t="shared" si="10"/>
+        <v>4.75</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="11"/>
+        <v>5.25</v>
+      </c>
+      <c r="F26" s="2">
+        <v>5</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>3.11</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="2">
+        <f>0.9*F27</f>
+        <v>0.28800000000000003</v>
+      </c>
+      <c r="E27" s="2">
+        <f>1.1*F27</f>
+        <v>0.35200000000000004</v>
+      </c>
+      <c r="F27" s="2">
+        <v>0.32</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>3.12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="2">
+        <f>0.9*F28</f>
+        <v>0.6120000000000001</v>
+      </c>
+      <c r="E28" s="2">
+        <f>1.1*F28</f>
+        <v>0.74800000000000011</v>
+      </c>
+      <c r="F28" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>3.13</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" ref="D29:D31" si="12">0.9*F29</f>
+        <v>0.9900000000000001</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" ref="E29:E31" si="13">1.1*F29</f>
+        <v>1.2100000000000002</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>3.14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="12"/>
+        <v>1.35</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="13"/>
+        <v>1.6500000000000001</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3.15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" si="12"/>
+        <v>1.71</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="13"/>
+        <v>2.09</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>4.01</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2">
+        <f t="shared" si="10"/>
+        <v>5.89</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="11"/>
+        <v>6.5100000000000007</v>
+      </c>
+      <c r="F32" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="B33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2">
+        <f t="shared" si="10"/>
+        <v>11.685</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="11"/>
+        <v>12.915000000000001</v>
+      </c>
+      <c r="F33" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>4.03</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="2">
+        <f t="shared" si="10"/>
+        <v>17.479999999999997</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="11"/>
+        <v>19.32</v>
+      </c>
+      <c r="F34" s="2">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>4.04</v>
+      </c>
+      <c r="B35" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="2">
+        <f t="shared" si="10"/>
+        <v>23.179999999999996</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="11"/>
+        <v>25.62</v>
+      </c>
+      <c r="F35" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>4.05</v>
+      </c>
+      <c r="B36" t="s">
+        <v>67</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D36" s="2">
+        <f t="shared" si="10"/>
+        <v>28.88</v>
+      </c>
+      <c r="E36" s="2">
+        <f t="shared" si="11"/>
+        <v>31.919999999999998</v>
+      </c>
+      <c r="F36" s="2">
+        <v>30.4</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="B37" t="s">
+        <v>109</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="2">
+        <f t="shared" ref="D37" si="14">0.95*F37</f>
+        <v>0.95</v>
+      </c>
+      <c r="E37" s="2">
+        <f t="shared" ref="E37" si="15">1.05*F37</f>
+        <v>1.05</v>
+      </c>
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>4.07</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" s="2">
+        <f t="shared" ref="D38:D41" si="16">0.95*F38</f>
+        <v>1.9</v>
+      </c>
+      <c r="E38" s="2">
+        <f t="shared" ref="E38:E41" si="17">1.05*F38</f>
+        <v>2.1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>2</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>4.08</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="2">
+        <f t="shared" si="16"/>
+        <v>2.8499999999999996</v>
+      </c>
+      <c r="E39" s="2">
+        <f t="shared" si="17"/>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="F39" s="2">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>4.09</v>
+      </c>
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="2">
+        <f t="shared" si="16"/>
+        <v>3.8</v>
+      </c>
+      <c r="E40" s="2">
+        <f t="shared" si="17"/>
+        <v>4.2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="2">
+        <f t="shared" si="16"/>
+        <v>4.75</v>
+      </c>
+      <c r="E41" s="2">
+        <f t="shared" si="17"/>
+        <v>5.25</v>
+      </c>
+      <c r="F41" s="2">
+        <v>5</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>5.01</v>
+      </c>
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" s="2">
+        <v>999</v>
+      </c>
+      <c r="E42" s="2">
+        <v>9999999</v>
+      </c>
+      <c r="F42" s="2">
+        <v>999999</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="2">
+        <f t="shared" si="4"/>
+        <v>10.45</v>
+      </c>
+      <c r="E43" s="2">
+        <f t="shared" si="5"/>
+        <v>11.55</v>
+      </c>
+      <c r="F43" s="2">
+        <v>11</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>5.03</v>
+      </c>
+      <c r="B44" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="2">
+        <f t="shared" si="4"/>
+        <v>10.45</v>
+      </c>
+      <c r="E44" s="2">
+        <f t="shared" si="5"/>
+        <v>11.55</v>
+      </c>
+      <c r="F44" s="2">
+        <v>11</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>5.04</v>
+      </c>
+      <c r="B45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="2">
+        <f t="shared" si="4"/>
+        <v>10.45</v>
+      </c>
+      <c r="E45" s="2">
+        <f t="shared" si="5"/>
+        <v>11.55</v>
+      </c>
+      <c r="F45" s="2">
+        <v>11</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>6.01</v>
+      </c>
+      <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="F46" s="3">
+        <v>0</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>6.02</v>
+      </c>
+      <c r="B47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="2">
+        <f>0.9*F47</f>
+        <v>4.05</v>
+      </c>
+      <c r="E47" s="2">
+        <f>1.1*F47</f>
+        <v>4.95</v>
+      </c>
+      <c r="F47" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>6.03</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="F48" s="3">
+        <v>0</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>6.04</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="3">
+        <v>189</v>
+      </c>
+      <c r="E49" s="3">
+        <v>210</v>
+      </c>
+      <c r="F49" s="3">
+        <v>200</v>
+      </c>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>6.05</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="2">
+        <f>0.9*F50</f>
+        <v>4.05</v>
+      </c>
+      <c r="E50" s="2">
+        <f>1.1*F50</f>
+        <v>4.95</v>
+      </c>
+      <c r="F50" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>6.06</v>
+      </c>
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D51" s="3">
+        <v>189</v>
+      </c>
+      <c r="E51" s="3">
+        <v>210</v>
+      </c>
+      <c r="F51" s="3">
+        <v>200</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>6.07</v>
+      </c>
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>7.01</v>
+      </c>
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F53" s="3">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>7.02</v>
+      </c>
+      <c r="B54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F54" s="3">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>7.03</v>
+      </c>
+      <c r="B55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>7.04</v>
+      </c>
+      <c r="B56" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed instrument connection refresh on GUI selftester temp check fixed.  selftester other diodes implemented.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C4DDA9-E4ED-4936-AE93-FFFFB147F9B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71528876-8AC6-413D-BFCD-11CC438044C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4788" yWindow="288" windowWidth="16032" windowHeight="10800" firstSheet="4" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="6408" yWindow="1680" windowWidth="16032" windowHeight="10788" firstSheet="4" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="HWCheck" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="146">
   <si>
     <t>TEST #</t>
   </si>
@@ -474,6 +473,9 @@
   </si>
   <si>
     <t>Ribbon7</t>
+  </si>
+  <si>
+    <t>P/F</t>
   </si>
 </sst>
 </file>
@@ -4703,7 +4705,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4931,8 +4933,8 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G42" sqref="G42"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5509,12 +5511,12 @@
         <v>116</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" ref="D22" si="8">0.95*F22</f>
-        <v>0.95</v>
+        <f t="shared" ref="D22" si="8">0.9*F22</f>
+        <v>0.9</v>
       </c>
       <c r="E22" s="2">
-        <f t="shared" ref="E22" si="9">1.05*F22</f>
-        <v>1.05</v>
+        <f t="shared" ref="E22" si="9">1.1*F22</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
@@ -5535,12 +5537,12 @@
         <v>117</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:D36" si="10">0.95*F23</f>
-        <v>1.9</v>
+        <f t="shared" ref="D23:D26" si="10">0.9*F23</f>
+        <v>1.8</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" ref="E23:E36" si="11">1.05*F23</f>
-        <v>2.1</v>
+        <f t="shared" ref="E23:E26" si="11">1.1*F23</f>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F23" s="2">
         <v>2</v>
@@ -5562,11 +5564,11 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="10"/>
-        <v>2.8499999999999996</v>
+        <v>2.7</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="11"/>
-        <v>3.1500000000000004</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="F24" s="2">
         <v>3</v>
@@ -5588,11 +5590,11 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="10"/>
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="11"/>
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F25" s="2">
         <v>4</v>
@@ -5614,11 +5616,11 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="10"/>
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="11"/>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
       <c r="F26" s="2">
         <v>5</v>
@@ -5769,11 +5771,11 @@
         <v>45</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D32:D36" si="14">0.95*F32</f>
         <v>5.89</v>
       </c>
       <c r="E32" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="E32:E36" si="15">1.05*F32</f>
         <v>6.5100000000000007</v>
       </c>
       <c r="F32" s="2">
@@ -5795,11 +5797,11 @@
         <v>45</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>11.685</v>
       </c>
       <c r="E33" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>12.915000000000001</v>
       </c>
       <c r="F33" s="2">
@@ -5821,11 +5823,11 @@
         <v>45</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>17.479999999999997</v>
       </c>
       <c r="E34" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>19.32</v>
       </c>
       <c r="F34" s="2">
@@ -5847,11 +5849,11 @@
         <v>45</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>23.179999999999996</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>25.62</v>
       </c>
       <c r="F35" s="2">
@@ -5873,11 +5875,11 @@
         <v>45</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>28.88</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>31.919999999999998</v>
       </c>
       <c r="F36" s="2">
@@ -5899,12 +5901,12 @@
         <v>47</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" ref="D37" si="14">0.95*F37</f>
-        <v>0.95</v>
+        <f>0.9*F37</f>
+        <v>0.9</v>
       </c>
       <c r="E37" s="2">
-        <f t="shared" ref="E37" si="15">1.05*F37</f>
-        <v>1.05</v>
+        <f>1.1*F37</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F37" s="2">
         <v>1</v>
@@ -5925,12 +5927,12 @@
         <v>47</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" ref="D38:D41" si="16">0.95*F38</f>
-        <v>1.9</v>
+        <f t="shared" ref="D38:D41" si="16">0.9*F38</f>
+        <v>1.8</v>
       </c>
       <c r="E38" s="2">
-        <f t="shared" ref="E38:E41" si="17">1.05*F38</f>
-        <v>2.1</v>
+        <f t="shared" ref="E38:E41" si="17">1.1*F38</f>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F38" s="2">
         <v>2</v>
@@ -5952,11 +5954,11 @@
       </c>
       <c r="D39" s="2">
         <f t="shared" si="16"/>
-        <v>2.8499999999999996</v>
+        <v>2.7</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="17"/>
-        <v>3.1500000000000004</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="F39" s="2">
         <v>3</v>
@@ -5978,11 +5980,11 @@
       </c>
       <c r="D40" s="2">
         <f t="shared" si="16"/>
-        <v>3.8</v>
+        <v>3.6</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="17"/>
-        <v>4.2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F40" s="2">
         <v>4</v>
@@ -6004,11 +6006,11 @@
       </c>
       <c r="D41" s="2">
         <f t="shared" si="16"/>
-        <v>4.75</v>
+        <v>4.5</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="17"/>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
       <c r="F41" s="2">
         <v>5</v>
@@ -6184,7 +6186,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="3">
-        <v>1E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="F48" s="3">
         <v>0</v>
@@ -6255,13 +6257,13 @@
         <v>143</v>
       </c>
       <c r="D51" s="3">
-        <v>189</v>
+        <v>0</v>
       </c>
       <c r="E51" s="3">
-        <v>210</v>
+        <v>50</v>
       </c>
       <c r="F51" s="3">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3" t="s">
@@ -6278,14 +6280,16 @@
       <c r="C52" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D52" s="3">
-        <v>0</v>
-      </c>
-      <c r="E52" s="3">
-        <v>1E-3</v>
+      <c r="D52" s="2">
+        <f>0.9*F52</f>
+        <v>4.05</v>
+      </c>
+      <c r="E52" s="2">
+        <f>1.1*F52</f>
+        <v>4.95</v>
       </c>
       <c r="F52" s="3">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3" t="s">
@@ -6312,7 +6316,9 @@
         <v>1</v>
       </c>
       <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
+      <c r="H53" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
@@ -6334,7 +6340,9 @@
         <v>1</v>
       </c>
       <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
+      <c r="H54" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
@@ -6355,6 +6363,9 @@
       <c r="F55" s="3">
         <v>1</v>
       </c>
+      <c r="H55" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
@@ -6374,6 +6385,9 @@
       </c>
       <c r="F56" s="3">
         <v>1</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more identifyable failure notes for debug in Tester.py during UVLO/OVLO
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71528876-8AC6-413D-BFCD-11CC438044C7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D67F8-DCA8-4200-82A7-57028FBBA0AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6408" yWindow="1680" windowWidth="16032" windowHeight="10788" firstSheet="4" activeTab="7" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="432" yWindow="1152" windowWidth="16032" windowHeight="10788" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -839,15 +839,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CA788C9-474B-4068-A04A-775EAB4B4CD4}">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18.88671875" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="10.5546875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
@@ -1111,14 +1113,16 @@
       <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="3">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3">
-        <v>1E-3</v>
+      <c r="D10" s="2">
+        <f>0.9*F10</f>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E10" s="2">
+        <f>1.1*F10</f>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F10" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
@@ -1136,14 +1140,16 @@
       <c r="C11" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3">
-        <v>1E-3</v>
+      <c r="D11" s="2">
+        <f t="shared" ref="D11:D15" si="3">0.9*F11</f>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" ref="E11:E15" si="4">1.1*F11</f>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F11" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
@@ -1161,14 +1167,16 @@
       <c r="C12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3">
-        <v>0</v>
-      </c>
-      <c r="E12" s="3">
-        <v>1E-3</v>
+      <c r="D12" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F12" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
@@ -1186,14 +1194,16 @@
       <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="3">
-        <v>0</v>
-      </c>
-      <c r="E13" s="3">
-        <v>1E-3</v>
+      <c r="D13" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F13" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
@@ -1211,14 +1221,16 @@
       <c r="C14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="3">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1E-3</v>
+      <c r="D14" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
@@ -1236,14 +1248,16 @@
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="3">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1E-3</v>
+      <c r="D15" s="2">
+        <f t="shared" si="3"/>
+        <v>7.2000000000000007E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000005E-3</v>
       </c>
       <c r="F15" s="3">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
@@ -1311,7 +1325,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <f t="shared" ref="A18:A29" si="3">A17+0.01</f>
+        <f t="shared" ref="A18:A29" si="5">A17+0.01</f>
         <v>15.03</v>
       </c>
       <c r="B18" t="s">
@@ -1341,7 +1355,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.04</v>
       </c>
       <c r="B19" t="s">
@@ -1371,7 +1385,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.049999999999999</v>
       </c>
       <c r="B20" t="s">
@@ -1401,7 +1415,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.059999999999999</v>
       </c>
       <c r="B21" t="s">
@@ -1431,7 +1445,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.069999999999999</v>
       </c>
       <c r="B22" t="s">
@@ -1461,7 +1475,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.079999999999998</v>
       </c>
       <c r="B23" t="s">
@@ -1491,7 +1505,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.089999999999998</v>
       </c>
       <c r="B24" t="s">
@@ -1521,7 +1535,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.099999999999998</v>
       </c>
       <c r="B25" t="s">
@@ -1551,7 +1565,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.109999999999998</v>
       </c>
       <c r="B26" t="s">
@@ -1611,7 +1625,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.129999999999997</v>
       </c>
       <c r="B28" t="s">
@@ -1641,7 +1655,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>15.139999999999997</v>
       </c>
       <c r="B29" t="s">
@@ -1819,7 +1833,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <f t="shared" ref="A35:A46" si="4">A34+0.01</f>
+        <f t="shared" ref="A35:A46" si="6">A34+0.01</f>
         <v>17.030000000000005</v>
       </c>
       <c r="B35" t="s">
@@ -1849,7 +1863,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.040000000000006</v>
       </c>
       <c r="B36" t="s">
@@ -1879,7 +1893,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.050000000000008</v>
       </c>
       <c r="B37" t="s">
@@ -1909,7 +1923,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.060000000000009</v>
       </c>
       <c r="B38" t="s">
@@ -1939,7 +1953,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.070000000000011</v>
       </c>
       <c r="B39" t="s">
@@ -1969,7 +1983,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.080000000000013</v>
       </c>
       <c r="B40" t="s">
@@ -1999,7 +2013,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.090000000000014</v>
       </c>
       <c r="B41" t="s">
@@ -2029,7 +2043,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.100000000000016</v>
       </c>
       <c r="B42" t="s">
@@ -2059,7 +2073,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.110000000000017</v>
       </c>
       <c r="B43" t="s">
@@ -2089,7 +2103,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.120000000000019</v>
       </c>
       <c r="B44" t="s">
@@ -2119,7 +2133,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.13000000000002</v>
       </c>
       <c r="B45" t="s">
@@ -2149,7 +2163,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>17.140000000000022</v>
       </c>
       <c r="B46" t="s">
@@ -2238,7 +2252,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
-        <f t="shared" ref="A49:A61" si="5">A48+0.01</f>
+        <f t="shared" ref="A49:A61" si="7">A48+0.01</f>
         <v>18.030000000000005</v>
       </c>
       <c r="B49" t="s">
@@ -2268,7 +2282,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.040000000000006</v>
       </c>
       <c r="B50" t="s">
@@ -2298,7 +2312,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.050000000000008</v>
       </c>
       <c r="B51" t="s">
@@ -2328,7 +2342,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.060000000000009</v>
       </c>
       <c r="B52" t="s">
@@ -2358,7 +2372,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.070000000000011</v>
       </c>
       <c r="B53" t="s">
@@ -2388,7 +2402,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.080000000000013</v>
       </c>
       <c r="B54" t="s">
@@ -2418,7 +2432,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.090000000000014</v>
       </c>
       <c r="B55" t="s">
@@ -2448,7 +2462,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.100000000000016</v>
       </c>
       <c r="B56" t="s">
@@ -2478,7 +2492,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.110000000000017</v>
       </c>
       <c r="B57" t="s">
@@ -2508,7 +2522,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.120000000000019</v>
       </c>
       <c r="B58" t="s">
@@ -2538,7 +2552,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.13000000000002</v>
       </c>
       <c r="B59" t="s">
@@ -2568,7 +2582,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.140000000000022</v>
       </c>
       <c r="B60" t="s">
@@ -2598,7 +2612,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>18.150000000000023</v>
       </c>
       <c r="B61" t="s">
@@ -2687,7 +2701,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <f t="shared" ref="A64:A75" si="6">A63+0.01</f>
+        <f t="shared" ref="A64:A75" si="8">A63+0.01</f>
         <v>19.030000000000005</v>
       </c>
       <c r="B64" t="s">
@@ -2717,7 +2731,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.040000000000006</v>
       </c>
       <c r="B65" t="s">
@@ -2747,7 +2761,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.050000000000008</v>
       </c>
       <c r="B66" t="s">
@@ -2777,7 +2791,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.060000000000009</v>
       </c>
       <c r="B67" t="s">
@@ -2807,7 +2821,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.070000000000011</v>
       </c>
       <c r="B68" t="s">
@@ -2837,7 +2851,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.080000000000013</v>
       </c>
       <c r="B69" t="s">
@@ -2867,7 +2881,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.090000000000014</v>
       </c>
       <c r="B70" t="s">
@@ -2897,7 +2911,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.100000000000016</v>
       </c>
       <c r="B71" t="s">
@@ -2927,7 +2941,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.110000000000017</v>
       </c>
       <c r="B72" t="s">
@@ -2957,7 +2971,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.120000000000019</v>
       </c>
       <c r="B73" t="s">
@@ -2987,7 +3001,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.13000000000002</v>
       </c>
       <c r="B74" t="s">
@@ -3017,7 +3031,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>19.140000000000022</v>
       </c>
       <c r="B75" t="s">
@@ -3106,7 +3120,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
-        <f t="shared" ref="A78:A80" si="7">A77+0.01</f>
+        <f t="shared" ref="A78:A80" si="9">A77+0.01</f>
         <v>20.030000000000005</v>
       </c>
       <c r="B78" t="s">
@@ -3136,7 +3150,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20.040000000000006</v>
       </c>
       <c r="B79" t="s">
@@ -3166,7 +3180,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>20.050000000000008</v>
       </c>
       <c r="B80" t="s">
@@ -3255,7 +3269,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
-        <f t="shared" ref="A83:A95" si="8">A82+0.01</f>
+        <f t="shared" ref="A83:A95" si="10">A82+0.01</f>
         <v>21.030000000000005</v>
       </c>
       <c r="B83" t="s">
@@ -3285,7 +3299,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.040000000000006</v>
       </c>
       <c r="B84" t="s">
@@ -3315,7 +3329,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.050000000000008</v>
       </c>
       <c r="B85" t="s">
@@ -3345,7 +3359,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.060000000000009</v>
       </c>
       <c r="B86" t="s">
@@ -3375,7 +3389,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.070000000000011</v>
       </c>
       <c r="B87" t="s">
@@ -3405,7 +3419,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.080000000000013</v>
       </c>
       <c r="B88" t="s">
@@ -3435,7 +3449,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.090000000000014</v>
       </c>
       <c r="B89" t="s">
@@ -3465,7 +3479,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.100000000000016</v>
       </c>
       <c r="B90" t="s">
@@ -3495,7 +3509,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.110000000000017</v>
       </c>
       <c r="B91" t="s">
@@ -3525,7 +3539,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.120000000000019</v>
       </c>
       <c r="B92" t="s">
@@ -3555,7 +3569,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.13000000000002</v>
       </c>
       <c r="B93" t="s">
@@ -3585,7 +3599,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.140000000000022</v>
       </c>
       <c r="B94" t="s">
@@ -3615,7 +3629,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>21.150000000000023</v>
       </c>
       <c r="B95" t="s">
@@ -4932,8 +4946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB3A8150-0F2A-4305-BFC4-9E49C077B26A}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated TP2B spec values during power off mode.  fixed ramp rate bug during test.  Test is ready for release!
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D67F8-DCA8-4200-82A7-57028FBBA0AB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BFDB17-9021-408A-9158-7EE6FF4BE89C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="432" yWindow="1152" windowWidth="16032" windowHeight="10788" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -840,8 +840,8 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,7 +1325,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <f t="shared" ref="A18:A29" si="5">A17+0.01</f>
+        <f t="shared" ref="A18:A26" si="5">A17+0.01</f>
         <v>15.03</v>
       </c>
       <c r="B18" t="s">
@@ -1625,7 +1625,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <f t="shared" si="5"/>
+        <f>A27+0.01</f>
         <v>15.129999999999997</v>
       </c>
       <c r="B28" t="s">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="E28" s="3">
         <f>NoPowerState!C14</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F28" s="3">
         <f>NoPowerState!D14</f>
@@ -1655,7 +1655,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <f t="shared" si="5"/>
+        <f>A28+0.01</f>
         <v>15.139999999999997</v>
       </c>
       <c r="B29" t="s">
@@ -2701,7 +2701,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
-        <f t="shared" ref="A64:A75" si="8">A63+0.01</f>
+        <f t="shared" ref="A64:A73" si="8">A63+0.01</f>
         <v>19.030000000000005</v>
       </c>
       <c r="B64" t="s">
@@ -3001,7 +3001,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
-        <f t="shared" si="8"/>
+        <f>A73+0.01</f>
         <v>19.13000000000002</v>
       </c>
       <c r="B74" t="s">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="E74" s="3">
         <f>NoPowerState!C14</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F74" s="3">
         <f>NoPowerState!D14</f>
@@ -3031,7 +3031,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
-        <f t="shared" si="8"/>
+        <f>A74+0.01</f>
         <v>19.140000000000022</v>
       </c>
       <c r="B75" t="s">
@@ -3668,7 +3668,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3905,7 +3905,7 @@
         <v>-0.5</v>
       </c>
       <c r="C14" s="3">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
increased limit for TP2B due to AKP findings.
</commit_message>
<xml_diff>
--- a/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
+++ b/PWRAutomatedTest/385-0030-TestSet/PWR_Board_TestReportTemplate2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ivan Moon\Documents\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\git\pluto\PWRAutomatedTest\385-0030-TestSet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE14823A-70D2-455C-A876-7C0F05D8F884}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3498180-33FF-4D63-8F1E-D795CC99F1B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
+    <workbookView xWindow="-19320" yWindow="720" windowWidth="19440" windowHeight="15600" xr2:uid="{4A8DB9E0-1329-4CE1-A68A-3922F0D4E040}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -840,22 +840,22 @@
   <dimension ref="A1:J95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10:E15"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -887,7 +887,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -913,7 +913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>1+A2</f>
         <v>2</v>
@@ -940,7 +940,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A15" si="2">1+A3</f>
         <v>3</v>
@@ -967,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -994,7 +994,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="2"/>
         <v>5</v>
@@ -1021,7 +1021,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="2"/>
         <v>6</v>
@@ -1048,7 +1048,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="2"/>
         <v>7</v>
@@ -1075,7 +1075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="2"/>
         <v>8</v>
@@ -1102,7 +1102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="2"/>
         <v>9</v>
@@ -1129,7 +1129,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="2"/>
         <v>10</v>
@@ -1156,7 +1156,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="2"/>
         <v>11</v>
@@ -1183,7 +1183,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="2"/>
         <v>12</v>
@@ -1210,7 +1210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="2"/>
         <v>13</v>
@@ -1237,7 +1237,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -1264,7 +1264,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15.01</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f>A16+0.01</f>
         <v>15.02</v>
@@ -1323,7 +1323,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" ref="A18:A26" si="5">A17+0.01</f>
         <v>15.03</v>
@@ -1353,7 +1353,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="5"/>
         <v>15.04</v>
@@ -1383,7 +1383,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="5"/>
         <v>15.049999999999999</v>
@@ -1413,7 +1413,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="5"/>
         <v>15.059999999999999</v>
@@ -1443,7 +1443,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="5"/>
         <v>15.069999999999999</v>
@@ -1473,7 +1473,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="5"/>
         <v>15.079999999999998</v>
@@ -1503,7 +1503,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="5"/>
         <v>15.089999999999998</v>
@@ -1533,7 +1533,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="5"/>
         <v>15.099999999999998</v>
@@ -1563,7 +1563,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="5"/>
         <v>15.109999999999998</v>
@@ -1593,7 +1593,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f>A26+0.01</f>
         <v>15.119999999999997</v>
@@ -1623,7 +1623,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f>A27+0.01</f>
         <v>15.129999999999997</v>
@@ -1653,7 +1653,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f>A28+0.01</f>
         <v>15.139999999999997</v>
@@ -1683,7 +1683,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>16.010000000000002</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f>A30+0.01</f>
         <v>16.020000000000003</v>
@@ -1742,7 +1742,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f>A31+0.01</f>
         <v>16.030000000000005</v>
@@ -1760,7 +1760,7 @@
       </c>
       <c r="E32" s="3">
         <f>CapsChargingState!C4</f>
-        <v>26.2</v>
+        <v>28</v>
       </c>
       <c r="F32" s="3">
         <f>CapsChargingState!D4</f>
@@ -1772,7 +1772,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>17.010000000000002</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f>A33+0.01</f>
         <v>17.020000000000003</v>
@@ -1831,7 +1831,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" ref="A35:A46" si="6">A34+0.01</f>
         <v>17.030000000000005</v>
@@ -1861,7 +1861,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="6"/>
         <v>17.040000000000006</v>
@@ -1891,7 +1891,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="6"/>
         <v>17.050000000000008</v>
@@ -1921,7 +1921,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="6"/>
         <v>17.060000000000009</v>
@@ -1951,7 +1951,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="6"/>
         <v>17.070000000000011</v>
@@ -1981,7 +1981,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="6"/>
         <v>17.080000000000013</v>
@@ -2011,7 +2011,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="6"/>
         <v>17.090000000000014</v>
@@ -2041,7 +2041,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="6"/>
         <v>17.100000000000016</v>
@@ -2071,7 +2071,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="6"/>
         <v>17.110000000000017</v>
@@ -2101,7 +2101,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="6"/>
         <v>17.120000000000019</v>
@@ -2131,7 +2131,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="6"/>
         <v>17.13000000000002</v>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="E45" s="3">
         <f>NormalOperationState!C14</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F45" s="3">
         <f>NormalOperationState!D14</f>
@@ -2161,7 +2161,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="6"/>
         <v>17.140000000000022</v>
@@ -2191,7 +2191,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>18.010000000000002</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f>A47+0.01</f>
         <v>18.020000000000003</v>
@@ -2250,7 +2250,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" ref="A49:A61" si="7">A48+0.01</f>
         <v>18.030000000000005</v>
@@ -2280,7 +2280,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="7"/>
         <v>18.040000000000006</v>
@@ -2310,7 +2310,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="7"/>
         <v>18.050000000000008</v>
@@ -2340,7 +2340,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="7"/>
         <v>18.060000000000009</v>
@@ -2370,7 +2370,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="7"/>
         <v>18.070000000000011</v>
@@ -2400,7 +2400,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="7"/>
         <v>18.080000000000013</v>
@@ -2430,7 +2430,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="7"/>
         <v>18.090000000000014</v>
@@ -2460,7 +2460,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="7"/>
         <v>18.100000000000016</v>
@@ -2490,7 +2490,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="7"/>
         <v>18.110000000000017</v>
@@ -2520,7 +2520,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="7"/>
         <v>18.120000000000019</v>
@@ -2550,7 +2550,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="7"/>
         <v>18.13000000000002</v>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="E59" s="3">
         <f>SPMState!C14</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F59" s="3">
         <f>SPMState!D14</f>
@@ -2580,7 +2580,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="7"/>
         <v>18.140000000000022</v>
@@ -2610,7 +2610,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="7"/>
         <v>18.150000000000023</v>
@@ -2640,7 +2640,7 @@
         <v>%</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>19.010000000000002</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f>A62+0.01</f>
         <v>19.020000000000003</v>
@@ -2699,7 +2699,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" ref="A64:A73" si="8">A63+0.01</f>
         <v>19.030000000000005</v>
@@ -2729,7 +2729,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="8"/>
         <v>19.040000000000006</v>
@@ -2759,7 +2759,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="8"/>
         <v>19.050000000000008</v>
@@ -2789,7 +2789,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="8"/>
         <v>19.060000000000009</v>
@@ -2819,7 +2819,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="8"/>
         <v>19.070000000000011</v>
@@ -2849,7 +2849,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" si="8"/>
         <v>19.080000000000013</v>
@@ -2879,7 +2879,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="8"/>
         <v>19.090000000000014</v>
@@ -2909,7 +2909,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="8"/>
         <v>19.100000000000016</v>
@@ -2939,7 +2939,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="8"/>
         <v>19.110000000000017</v>
@@ -2969,7 +2969,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="8"/>
         <v>19.120000000000019</v>
@@ -2999,7 +2999,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f>A73+0.01</f>
         <v>19.13000000000002</v>
@@ -3029,7 +3029,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f>A74+0.01</f>
         <v>19.140000000000022</v>
@@ -3059,7 +3059,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>20.010000000000002</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f>A76+0.01</f>
         <v>20.020000000000003</v>
@@ -3118,7 +3118,7 @@
         <v>dv/dt</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" ref="A78:A80" si="9">A77+0.01</f>
         <v>20.030000000000005</v>
@@ -3148,7 +3148,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="9"/>
         <v>20.040000000000006</v>
@@ -3178,7 +3178,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="9"/>
         <v>20.050000000000008</v>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="E80" s="3">
         <f>BootstrapState!C6</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F80" s="3">
         <f>BootstrapState!D6</f>
@@ -3208,7 +3208,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>21.01</v>
       </c>
@@ -3237,7 +3237,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f>A81+0.01</f>
         <v>21.020000000000003</v>
@@ -3267,7 +3267,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" ref="A83:A95" si="10">A82+0.01</f>
         <v>21.030000000000005</v>
@@ -3297,7 +3297,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="10"/>
         <v>21.040000000000006</v>
@@ -3327,7 +3327,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="10"/>
         <v>21.050000000000008</v>
@@ -3357,7 +3357,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="10"/>
         <v>21.060000000000009</v>
@@ -3387,7 +3387,7 @@
         <v>degC</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="10"/>
         <v>21.070000000000011</v>
@@ -3417,7 +3417,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="10"/>
         <v>21.080000000000013</v>
@@ -3447,7 +3447,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="10"/>
         <v>21.090000000000014</v>
@@ -3477,7 +3477,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="10"/>
         <v>21.100000000000016</v>
@@ -3507,7 +3507,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="10"/>
         <v>21.110000000000017</v>
@@ -3537,7 +3537,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="10"/>
         <v>21.120000000000019</v>
@@ -3567,7 +3567,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="10"/>
         <v>21.13000000000002</v>
@@ -3585,7 +3585,7 @@
       </c>
       <c r="E93" s="3">
         <f>SPMState!C14</f>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F93" s="3">
         <f>SPMState!D14</f>
@@ -3597,7 +3597,7 @@
         <v>V</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="10"/>
         <v>21.140000000000022</v>
@@ -3627,7 +3627,7 @@
         <v>A</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <f t="shared" si="10"/>
         <v>21.150000000000023</v>
@@ -3671,12 +3671,12 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3693,7 +3693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -3744,7 +3744,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -3812,7 +3812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -3846,7 +3846,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3941,15 +3941,15 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4085,7 +4085,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4119,7 +4119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4136,7 +4136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4153,7 +4153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4170,7 +4170,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3">
         <v>24</v>
@@ -4187,7 +4187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4214,12 +4214,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4236,7 +4236,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -4253,7 +4253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4278,7 +4278,7 @@
         <v>23.8</v>
       </c>
       <c r="C4" s="3">
-        <v>26.2</v>
+        <v>28</v>
       </c>
       <c r="D4" s="3">
         <v>25</v>
@@ -4297,17 +4297,17 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4536,7 +4536,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14" s="3">
         <v>24</v>
@@ -4545,7 +4545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -4589,15 +4589,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -4614,7 +4614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
@@ -4682,7 +4682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3">
         <v>20</v>
@@ -4699,12 +4699,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -4722,12 +4722,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -4825,7 +4825,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>44</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -4895,7 +4895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>47</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -4951,18 +4951,18 @@
       <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.21875" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4994,7 +4994,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.01</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.02</v>
       </c>
@@ -5046,7 +5046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.03</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.04</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.05</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.0099999999999998</v>
       </c>
@@ -5150,7 +5150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2.02</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2.0299999999999998</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.04</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2.0499999999999998</v>
       </c>
@@ -5254,7 +5254,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2.06</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2.0699999999999998</v>
       </c>
@@ -5306,7 +5306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2.08</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2.09</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2.1</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3.01</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3.02</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3.03</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3.04</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3.05</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3.06</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3.07</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.08</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.09</v>
       </c>
@@ -5618,7 +5618,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.1</v>
       </c>
@@ -5644,7 +5644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3.11</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3.12</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>3.13</v>
       </c>
@@ -5722,7 +5722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3.14</v>
       </c>
@@ -5748,7 +5748,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>3.15</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.01</v>
       </c>
@@ -5800,7 +5800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4.0199999999999996</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>4.03</v>
       </c>
@@ -5852,7 +5852,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4.04</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4.05</v>
       </c>
@@ -5904,7 +5904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4.0599999999999996</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4.07</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>4.08</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4.09</v>
       </c>
@@ -6008,7 +6008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4.0999999999999996</v>
       </c>
@@ -6034,7 +6034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5.01</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>5.0199999999999996</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5.03</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>5.04</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>6.01</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>6.02</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>6.03</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6.04</v>
       </c>
@@ -6234,7 +6234,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>6.05</v>
       </c>
@@ -6260,7 +6260,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6.06</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>6.07</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>7.01</v>
       </c>
@@ -6334,7 +6334,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>7.02</v>
       </c>
@@ -6358,7 +6358,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7.03</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7.04</v>
       </c>

</xml_diff>